<commit_message>
added data to exel file
</commit_message>
<xml_diff>
--- a/Output/Kernel vergleich.xlsx
+++ b/Output/Kernel vergleich.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Moritz\Documents\Bachelorarbeit code\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Moritz\Documents\Bachelorarbeit\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="19">
   <si>
     <t>AMD</t>
   </si>
@@ -79,6 +79,9 @@
   <si>
     <t>work dim 1 and local work size 64 with loading to local mem</t>
   </si>
+  <si>
+    <t>Dynamic</t>
+  </si>
 </sst>
 </file>
 
@@ -116,7 +119,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -135,6 +138,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -258,13 +264,13 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Tabelle1!$B$6:$B$22</c15:sqref>
+                    <c15:sqref>Tabelle1!$B$6:$B$25</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Tabelle1!$B$6,Tabelle1!$B$9,Tabelle1!$B$12,Tabelle1!$B$15,Tabelle1!$B$18,Tabelle1!$B$21)</c:f>
+              <c:f>(Tabelle1!$B$6,Tabelle1!$B$9,Tabelle1!$B$12,Tabelle1!$B$15,Tabelle1!$B$18,Tabelle1!$B$21,Tabelle1!$B$24)</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -282,6 +288,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>4.2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Dynamic</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -291,14 +300,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Tabelle1!$E$6:$E$22</c15:sqref>
+                    <c15:sqref>Tabelle1!$E$6:$E$25</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Tabelle1!$E$6,Tabelle1!$E$9,Tabelle1!$E$12,Tabelle1!$E$15,Tabelle1!$E$18,Tabelle1!$E$21)</c:f>
+              <c:f>(Tabelle1!$E$6,Tabelle1!$E$9,Tabelle1!$E$12,Tabelle1!$E$15,Tabelle1!$E$18,Tabelle1!$E$21,Tabelle1!$E$24)</c:f>
               <c:numCache>
-                <c:formatCode>0.00000</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:formatCode>000,000</c:formatCode>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>19.013000000000002</c:v>
                 </c:pt>
@@ -316,6 +325,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>2.954555</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>2.9246574999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -331,8 +343,8 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-352080816"/>
-        <c:axId val="-352075920"/>
+        <c:axId val="-1821523632"/>
+        <c:axId val="-1821537232"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredBarSeries>
@@ -371,15 +383,15 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>Tabelle1!$B$6:$B$22</c15:sqref>
+                          <c15:sqref>Tabelle1!$B$6:$B$25</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(Tabelle1!$B$6,Tabelle1!$B$9,Tabelle1!$B$12,Tabelle1!$B$15,Tabelle1!$B$18,Tabelle1!$B$21)</c15:sqref>
+                          <c15:sqref>(Tabelle1!$B$6,Tabelle1!$B$9,Tabelle1!$B$12,Tabelle1!$B$15,Tabelle1!$B$18,Tabelle1!$B$21,Tabelle1!$B$24)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:strCache>
-                      <c:ptCount val="6"/>
+                      <c:ptCount val="7"/>
                       <c:pt idx="0">
                         <c:v>1</c:v>
                       </c:pt>
@@ -397,6 +409,12 @@
                       </c:pt>
                       <c:pt idx="5">
                         <c:v>4.2</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>Dynamic</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>Dynamic</c:v>
                       </c:pt>
                     </c:strCache>
                   </c:strRef>
@@ -445,7 +463,7 @@
                 <c:order val="1"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Tabelle1!$D$5</c15:sqref>
@@ -475,15 +493,15 @@
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>Tabelle1!$B$6:$B$22</c15:sqref>
+                          <c15:sqref>Tabelle1!$B$6:$B$25</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(Tabelle1!$B$6,Tabelle1!$B$9,Tabelle1!$B$12,Tabelle1!$B$15,Tabelle1!$B$18,Tabelle1!$B$21)</c15:sqref>
+                          <c15:sqref>(Tabelle1!$B$6,Tabelle1!$B$9,Tabelle1!$B$12,Tabelle1!$B$15,Tabelle1!$B$18,Tabelle1!$B$21,Tabelle1!$B$24)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:strCache>
-                      <c:ptCount val="6"/>
+                      <c:ptCount val="7"/>
                       <c:pt idx="0">
                         <c:v>1</c:v>
                       </c:pt>
@@ -501,6 +519,9 @@
                       </c:pt>
                       <c:pt idx="5">
                         <c:v>4.2</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>Dynamic</c:v>
                       </c:pt>
                     </c:strCache>
                   </c:strRef>
@@ -510,33 +531,36 @@
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>Tabelle1!$D$6:$D$22</c15:sqref>
+                          <c15:sqref>Tabelle1!$E$6:$E$25</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(Tabelle1!$D$6,Tabelle1!$D$9,Tabelle1!$D$12,Tabelle1!$D$15,Tabelle1!$D$18,Tabelle1!$D$21)</c15:sqref>
+                          <c15:sqref>(Tabelle1!$E$6,Tabelle1!$E$9,Tabelle1!$E$12,Tabelle1!$E$15,Tabelle1!$E$18,Tabelle1!$E$21,Tabelle1!$E$24)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>0.00000</c:formatCode>
-                      <c:ptCount val="6"/>
+                      <c:ptCount val="7"/>
                       <c:pt idx="0">
-                        <c:v>8.1672499999999992</c:v>
+                        <c:v>19.013000000000002</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>0</c:v>
+                        <c:v>0.77977624999999995</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>0.69224300000000005</c:v>
+                        <c:v>2.15306</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>0</c:v>
+                        <c:v>1.1096766666666669</c:v>
                       </c:pt>
                       <c:pt idx="4">
-                        <c:v>0</c:v>
+                        <c:v>0.84413766666666668</c:v>
                       </c:pt>
                       <c:pt idx="5">
-                        <c:v>0</c:v>
+                        <c:v>2.954555</c:v>
+                      </c:pt>
+                      <c:pt idx="6" formatCode="General">
+                        <c:v>2.9246574999999999</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -547,7 +571,7 @@
         </c:extLst>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-352080816"/>
+        <c:axId val="-1821523632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -590,7 +614,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-352075920"/>
+        <c:crossAx val="-1821537232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -598,7 +622,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-352075920"/>
+        <c:axId val="-1821537232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="20"/>
@@ -652,7 +676,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-352080816"/>
+        <c:crossAx val="-1821523632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -847,13 +871,13 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Tabelle1!$B$6:$B$22</c15:sqref>
+                    <c15:sqref>Tabelle1!$B$6:$B$25</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Tabelle1!$B$6,Tabelle1!$B$9,Tabelle1!$B$12,Tabelle1!$B$15,Tabelle1!$B$18,Tabelle1!$B$21)</c:f>
+              <c:f>(Tabelle1!$B$6,Tabelle1!$B$9,Tabelle1!$B$12,Tabelle1!$B$15,Tabelle1!$B$18,Tabelle1!$B$21,Tabelle1!$B$24)</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -871,6 +895,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>4.2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Dynamic</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -880,31 +907,34 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Tabelle1!$C$6:$C$22</c15:sqref>
+                    <c15:sqref>Tabelle1!$C$6:$C$25</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Tabelle1!$C$6,Tabelle1!$C$9,Tabelle1!$C$12,Tabelle1!$C$15,Tabelle1!$C$18,Tabelle1!$C$21)</c:f>
+              <c:f>(Tabelle1!$C$6,Tabelle1!$C$9,Tabelle1!$C$12,Tabelle1!$C$15,Tabelle1!$C$18,Tabelle1!$C$21,Tabelle1!$C$24)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0" formatCode="0.00000">
+                <c:ptCount val="7"/>
+                <c:pt idx="0" formatCode="000,000">
                   <c:v>0.53157466669999998</c:v>
                 </c:pt>
-                <c:pt idx="1" formatCode="0.00000">
+                <c:pt idx="1" formatCode="000,000">
                   <c:v>0.43307000000000001</c:v>
                 </c:pt>
-                <c:pt idx="2" formatCode="0.00000">
+                <c:pt idx="2" formatCode="000,000">
                   <c:v>0.69523500000000005</c:v>
                 </c:pt>
-                <c:pt idx="3" formatCode="0.00000">
+                <c:pt idx="3" formatCode="000,000">
                   <c:v>1.0202374999999999</c:v>
                 </c:pt>
-                <c:pt idx="4" formatCode="0.00000">
+                <c:pt idx="4" formatCode="000,000">
                   <c:v>0.5261922</c:v>
                 </c:pt>
-                <c:pt idx="5" formatCode="0.00000">
+                <c:pt idx="5" formatCode="000,000">
                   <c:v>1.1054575</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.81096674999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -920,8 +950,8 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-521199392"/>
-        <c:axId val="-521191232"/>
+        <c:axId val="-2057977184"/>
+        <c:axId val="-2057974464"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredBarSeries>
@@ -960,15 +990,15 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>Tabelle1!$B$6:$B$22</c15:sqref>
+                          <c15:sqref>Tabelle1!$B$6:$B$25</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(Tabelle1!$B$6,Tabelle1!$B$9,Tabelle1!$B$12,Tabelle1!$B$15,Tabelle1!$B$18,Tabelle1!$B$21)</c15:sqref>
+                          <c15:sqref>(Tabelle1!$B$6,Tabelle1!$B$9,Tabelle1!$B$12,Tabelle1!$B$15,Tabelle1!$B$18,Tabelle1!$B$21,Tabelle1!$B$24)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:strCache>
-                      <c:ptCount val="6"/>
+                      <c:ptCount val="7"/>
                       <c:pt idx="0">
                         <c:v>1</c:v>
                       </c:pt>
@@ -986,6 +1016,12 @@
                       </c:pt>
                       <c:pt idx="5">
                         <c:v>4.2</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>Dynamic</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>Dynamic</c:v>
                       </c:pt>
                     </c:strCache>
                   </c:strRef>
@@ -1009,16 +1045,16 @@
                         <c:v>8.1672499999999992</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>0</c:v>
+                        <c:v>0.57916349999999994</c:v>
                       </c:pt>
                       <c:pt idx="2">
                         <c:v>0.69224300000000005</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>0</c:v>
+                        <c:v>0.65996350000000004</c:v>
                       </c:pt>
                       <c:pt idx="4">
-                        <c:v>0</c:v>
+                        <c:v>0.89916050000000003</c:v>
                       </c:pt>
                       <c:pt idx="5">
                         <c:v>0</c:v>
@@ -1034,7 +1070,7 @@
                 <c:order val="2"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Tabelle1!$E$5</c15:sqref>
@@ -1064,15 +1100,15 @@
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>Tabelle1!$B$6:$B$22</c15:sqref>
+                          <c15:sqref>Tabelle1!$B$6:$B$25</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(Tabelle1!$B$6,Tabelle1!$B$9,Tabelle1!$B$12,Tabelle1!$B$15,Tabelle1!$B$18,Tabelle1!$B$21)</c15:sqref>
+                          <c15:sqref>(Tabelle1!$B$6,Tabelle1!$B$9,Tabelle1!$B$12,Tabelle1!$B$15,Tabelle1!$B$18,Tabelle1!$B$21,Tabelle1!$B$24)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:strCache>
-                      <c:ptCount val="6"/>
+                      <c:ptCount val="7"/>
                       <c:pt idx="0">
                         <c:v>1</c:v>
                       </c:pt>
@@ -1090,6 +1126,12 @@
                       </c:pt>
                       <c:pt idx="5">
                         <c:v>4.2</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>Dynamic</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>Dynamic</c:v>
                       </c:pt>
                     </c:strCache>
                   </c:strRef>
@@ -1136,7 +1178,7 @@
         </c:extLst>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-521199392"/>
+        <c:axId val="-2057977184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1179,7 +1221,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-521191232"/>
+        <c:crossAx val="-2057974464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1187,7 +1229,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-521191232"/>
+        <c:axId val="-2057974464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1238,7 +1280,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-521199392"/>
+        <c:crossAx val="-2057977184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.1"/>
@@ -1433,13 +1475,13 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Tabelle1!$B$6:$B$22</c15:sqref>
+                    <c15:sqref>Tabelle1!$B$6:$B$25</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Tabelle1!$B$6,Tabelle1!$B$9,Tabelle1!$B$12,Tabelle1!$B$15,Tabelle1!$B$18,Tabelle1!$B$21)</c:f>
+              <c:f>(Tabelle1!$B$6,Tabelle1!$B$9,Tabelle1!$B$12,Tabelle1!$B$15,Tabelle1!$B$18,Tabelle1!$B$21,Tabelle1!$B$24)</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1457,6 +1499,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>4.2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Dynamic</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1466,31 +1511,34 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Tabelle1!$D$6:$D$22</c15:sqref>
+                    <c15:sqref>Tabelle1!$D$6:$D$25</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Tabelle1!$D$6,Tabelle1!$D$9,Tabelle1!$D$12,Tabelle1!$D$15,Tabelle1!$D$18,Tabelle1!$D$21)</c:f>
+              <c:f>(Tabelle1!$D$6,Tabelle1!$D$9,Tabelle1!$D$12,Tabelle1!$D$15,Tabelle1!$D$18,Tabelle1!$D$21,Tabelle1!$D$24)</c:f>
               <c:numCache>
-                <c:formatCode>0.00000</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:formatCode>000,000</c:formatCode>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>8.1672499999999992</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.57916349999999994</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.69224300000000005</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>0.65996350000000004</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>0.89916050000000003</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>0.91886025000000005</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1506,8 +1554,8 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-352088976"/>
-        <c:axId val="-521191776"/>
+        <c:axId val="-2003092800"/>
+        <c:axId val="-2003090080"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredBarSeries>
@@ -1546,15 +1594,15 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>Tabelle1!$B$6:$B$22</c15:sqref>
+                          <c15:sqref>Tabelle1!$B$6:$B$25</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(Tabelle1!$B$6,Tabelle1!$B$9,Tabelle1!$B$12,Tabelle1!$B$15,Tabelle1!$B$18,Tabelle1!$B$21)</c15:sqref>
+                          <c15:sqref>(Tabelle1!$B$6,Tabelle1!$B$9,Tabelle1!$B$12,Tabelle1!$B$15,Tabelle1!$B$18,Tabelle1!$B$21,Tabelle1!$B$24)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:strCache>
-                      <c:ptCount val="6"/>
+                      <c:ptCount val="7"/>
                       <c:pt idx="0">
                         <c:v>1</c:v>
                       </c:pt>
@@ -1572,6 +1620,12 @@
                       </c:pt>
                       <c:pt idx="5">
                         <c:v>4.2</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>Dynamic</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>Dynamic</c:v>
                       </c:pt>
                     </c:strCache>
                   </c:strRef>
@@ -1620,7 +1674,7 @@
                 <c:order val="2"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Tabelle1!$E$5</c15:sqref>
@@ -1650,15 +1704,15 @@
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>Tabelle1!$B$6:$B$22</c15:sqref>
+                          <c15:sqref>Tabelle1!$B$6:$B$25</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(Tabelle1!$B$6,Tabelle1!$B$9,Tabelle1!$B$12,Tabelle1!$B$15,Tabelle1!$B$18,Tabelle1!$B$21)</c15:sqref>
+                          <c15:sqref>(Tabelle1!$B$6,Tabelle1!$B$9,Tabelle1!$B$12,Tabelle1!$B$15,Tabelle1!$B$18,Tabelle1!$B$21,Tabelle1!$B$24)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:strCache>
-                      <c:ptCount val="6"/>
+                      <c:ptCount val="7"/>
                       <c:pt idx="0">
                         <c:v>1</c:v>
                       </c:pt>
@@ -1676,6 +1730,12 @@
                       </c:pt>
                       <c:pt idx="5">
                         <c:v>4.2</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>Dynamic</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>Dynamic</c:v>
                       </c:pt>
                     </c:strCache>
                   </c:strRef>
@@ -1722,7 +1782,7 @@
         </c:extLst>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-352088976"/>
+        <c:axId val="-2003092800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1765,7 +1825,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-521191776"/>
+        <c:crossAx val="-2003090080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1773,7 +1833,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-521191776"/>
+        <c:axId val="-2003090080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1824,7 +1884,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-352088976"/>
+        <c:crossAx val="-2003092800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -2002,7 +2062,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="FF0000"/>
+              <a:srgbClr val="00B050"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -2015,13 +2075,13 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Tabelle1!$B$6:$B$22</c15:sqref>
+                    <c15:sqref>Tabelle1!$B$6:$B$25</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Tabelle1!$B$6,Tabelle1!$B$9,Tabelle1!$B$12,Tabelle1!$B$15,Tabelle1!$B$18,Tabelle1!$B$21)</c:f>
+              <c:f>(Tabelle1!$B$6,Tabelle1!$B$9,Tabelle1!$B$12,Tabelle1!$B$15,Tabelle1!$B$18,Tabelle1!$B$21,Tabelle1!$B$24)</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -2039,6 +2099,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>4.2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Dynamic</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2048,14 +2111,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Tabelle1!$C$6:$C$22</c15:sqref>
+                    <c15:sqref>Tabelle1!$C$6:$C$25</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Tabelle1!$C$6,Tabelle1!$C$9,Tabelle1!$C$12,Tabelle1!$C$15,Tabelle1!$C$18,Tabelle1!$C$21)</c:f>
+              <c:f>(Tabelle1!$C$6,Tabelle1!$C$9,Tabelle1!$C$12,Tabelle1!$C$15,Tabelle1!$C$18,Tabelle1!$C$21,Tabelle1!$C$24)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0" formatCode="0.00000">
                   <c:v>0.53157466669999998</c:v>
                 </c:pt>
@@ -2073,6 +2136,9 @@
                 </c:pt>
                 <c:pt idx="5" formatCode="0.00000">
                   <c:v>1.1054575</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.81096674999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2107,13 +2173,13 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Tabelle1!$B$6:$B$22</c15:sqref>
+                    <c15:sqref>Tabelle1!$B$6:$B$25</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Tabelle1!$B$6,Tabelle1!$B$9,Tabelle1!$B$12,Tabelle1!$B$15,Tabelle1!$B$18,Tabelle1!$B$21)</c:f>
+              <c:f>(Tabelle1!$B$6,Tabelle1!$B$9,Tabelle1!$B$12,Tabelle1!$B$15,Tabelle1!$B$18,Tabelle1!$B$21,Tabelle1!$B$24)</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -2131,6 +2197,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>4.2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Dynamic</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2140,31 +2209,34 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Tabelle1!$D$6:$D$22</c15:sqref>
+                    <c15:sqref>Tabelle1!$D$6:$D$25</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Tabelle1!$D$6,Tabelle1!$D$9,Tabelle1!$D$12,Tabelle1!$D$15,Tabelle1!$D$18,Tabelle1!$D$21)</c:f>
+              <c:f>(Tabelle1!$D$6,Tabelle1!$D$9,Tabelle1!$D$12,Tabelle1!$D$15,Tabelle1!$D$18,Tabelle1!$D$21,Tabelle1!$D$24)</c:f>
               <c:numCache>
                 <c:formatCode>0.00000</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>8.1672499999999992</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.57916349999999994</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.69224300000000005</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>0.65996350000000004</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>0.89916050000000003</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>0.91886025000000005</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2186,7 +2258,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="00B050"/>
+              <a:srgbClr val="FF0000"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -2199,13 +2271,13 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Tabelle1!$B$6:$B$22</c15:sqref>
+                    <c15:sqref>Tabelle1!$B$6:$B$25</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Tabelle1!$B$6,Tabelle1!$B$9,Tabelle1!$B$12,Tabelle1!$B$15,Tabelle1!$B$18,Tabelle1!$B$21)</c:f>
+              <c:f>(Tabelle1!$B$6,Tabelle1!$B$9,Tabelle1!$B$12,Tabelle1!$B$15,Tabelle1!$B$18,Tabelle1!$B$21,Tabelle1!$B$24)</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -2223,6 +2295,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>4.2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Dynamic</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2232,14 +2307,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Tabelle1!$E$6:$E$22</c15:sqref>
+                    <c15:sqref>Tabelle1!$E$6:$E$25</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Tabelle1!$E$6,Tabelle1!$E$9,Tabelle1!$E$12,Tabelle1!$E$15,Tabelle1!$E$18,Tabelle1!$E$21)</c:f>
+              <c:f>(Tabelle1!$E$6,Tabelle1!$E$9,Tabelle1!$E$12,Tabelle1!$E$15,Tabelle1!$E$18,Tabelle1!$E$21,Tabelle1!$E$24)</c:f>
               <c:numCache>
-                <c:formatCode>0.00000</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:formatCode>000,000</c:formatCode>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>19.013000000000002</c:v>
                 </c:pt>
@@ -2257,6 +2332,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>2.954555</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>2.9246574999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2272,11 +2350,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-352085168"/>
-        <c:axId val="-352084624"/>
+        <c:axId val="-1738637936"/>
+        <c:axId val="-1738648816"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-352085168"/>
+        <c:axId val="-1738637936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2319,7 +2397,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-352084624"/>
+        <c:crossAx val="-1738648816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2327,7 +2405,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-352084624"/>
+        <c:axId val="-1738648816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2378,7 +2456,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-352085168"/>
+        <c:crossAx val="-1738637936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -2570,13 +2648,13 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Tabelle1!$B$6:$B$22</c15:sqref>
+                    <c15:sqref>Tabelle1!$B$6:$B$25</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Tabelle1!$B$7,Tabelle1!$B$10,Tabelle1!$B$13,Tabelle1!$B$16,Tabelle1!$B$19,Tabelle1!$B$22)</c:f>
+              <c:f>(Tabelle1!$B$7,Tabelle1!$B$10,Tabelle1!$B$13,Tabelle1!$B$16,Tabelle1!$B$19,Tabelle1!$B$22,Tabelle1!$B$25)</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -2594,6 +2672,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>4.2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Dynamic</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2603,14 +2684,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Tabelle1!$E$6:$E$22</c15:sqref>
+                    <c15:sqref>Tabelle1!$E$6:$E$25</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Tabelle1!$E$7,Tabelle1!$E$10,Tabelle1!$E$13,Tabelle1!$E$16,Tabelle1!$E$19,Tabelle1!$E$22)</c:f>
+              <c:f>(Tabelle1!$E$7,Tabelle1!$E$10,Tabelle1!$E$13,Tabelle1!$E$16,Tabelle1!$E$19,Tabelle1!$E$22,Tabelle1!$E$25)</c:f>
               <c:numCache>
                 <c:formatCode>0.00000</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>8.5662699999999994E-2</c:v>
                 </c:pt>
@@ -2628,6 +2709,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.75661400000000001</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>0.82827700000000004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2643,8 +2727,8 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-633254672"/>
-        <c:axId val="-633253040"/>
+        <c:axId val="-1738640656"/>
+        <c:axId val="-1738652624"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredBarSeries>
@@ -2683,15 +2767,15 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>Tabelle1!$B$6:$B$22</c15:sqref>
+                          <c15:sqref>Tabelle1!$B$6:$B$25</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(Tabelle1!$B$7,Tabelle1!$B$10,Tabelle1!$B$13,Tabelle1!$B$16,Tabelle1!$B$19,Tabelle1!$B$22)</c15:sqref>
+                          <c15:sqref>(Tabelle1!$B$7,Tabelle1!$B$10,Tabelle1!$B$13,Tabelle1!$B$16,Tabelle1!$B$19,Tabelle1!$B$22,Tabelle1!$B$25)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:strCache>
-                      <c:ptCount val="6"/>
+                      <c:ptCount val="7"/>
                       <c:pt idx="0">
                         <c:v>1</c:v>
                       </c:pt>
@@ -2709,6 +2793,12 @@
                       </c:pt>
                       <c:pt idx="5">
                         <c:v>4.2</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>Dynamic</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>Dynamic</c:v>
                       </c:pt>
                     </c:strCache>
                   </c:strRef>
@@ -2757,7 +2847,7 @@
                 <c:order val="1"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Tabelle1!$D$5</c15:sqref>
@@ -2787,15 +2877,15 @@
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>Tabelle1!$B$6:$B$22</c15:sqref>
+                          <c15:sqref>Tabelle1!$B$6:$B$25</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(Tabelle1!$B$7,Tabelle1!$B$10,Tabelle1!$B$13,Tabelle1!$B$16,Tabelle1!$B$19,Tabelle1!$B$22)</c15:sqref>
+                          <c15:sqref>(Tabelle1!$B$7,Tabelle1!$B$10,Tabelle1!$B$13,Tabelle1!$B$16,Tabelle1!$B$19,Tabelle1!$B$22,Tabelle1!$B$25)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:strCache>
-                      <c:ptCount val="6"/>
+                      <c:ptCount val="7"/>
                       <c:pt idx="0">
                         <c:v>1</c:v>
                       </c:pt>
@@ -2813,6 +2903,12 @@
                       </c:pt>
                       <c:pt idx="5">
                         <c:v>4.2</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>Dynamic</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>Dynamic</c:v>
                       </c:pt>
                     </c:strCache>
                   </c:strRef>
@@ -2836,16 +2932,16 @@
                         <c:v>0.21723400000000001</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>0</c:v>
+                        <c:v>3.3380874999999999</c:v>
                       </c:pt>
                       <c:pt idx="2">
                         <c:v>2.6963900000000001</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>0</c:v>
+                        <c:v>2.8530249999999997</c:v>
                       </c:pt>
                       <c:pt idx="4">
-                        <c:v>0</c:v>
+                        <c:v>2.0138775</c:v>
                       </c:pt>
                       <c:pt idx="5">
                         <c:v>0</c:v>
@@ -2859,7 +2955,7 @@
         </c:extLst>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-633254672"/>
+        <c:axId val="-1738640656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2902,7 +2998,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-633253040"/>
+        <c:crossAx val="-1738652624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2910,7 +3006,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-633253040"/>
+        <c:axId val="-1738652624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2961,7 +3057,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-633254672"/>
+        <c:crossAx val="-1738640656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.25"/>
@@ -3179,13 +3275,13 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Tabelle1!$B$6:$B$22</c15:sqref>
+                    <c15:sqref>Tabelle1!$B$6:$B$25</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Tabelle1!$B$7,Tabelle1!$B$10,Tabelle1!$B$13,Tabelle1!$B$16,Tabelle1!$B$19,Tabelle1!$B$22)</c:f>
+              <c:f>(Tabelle1!$B$7,Tabelle1!$B$10,Tabelle1!$B$13,Tabelle1!$B$16,Tabelle1!$B$19,Tabelle1!$B$22,Tabelle1!$B$25)</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -3203,6 +3299,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>4.2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Dynamic</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3212,31 +3311,34 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Tabelle1!$C$6:$C$22</c15:sqref>
+                    <c15:sqref>Tabelle1!$C$6:$C$25</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Tabelle1!$C$7,Tabelle1!$C$10,Tabelle1!$C$13,Tabelle1!$C$16,Tabelle1!$C$19,Tabelle1!$C$22)</c:f>
+              <c:f>(Tabelle1!$C$7,Tabelle1!$C$10,Tabelle1!$C$13,Tabelle1!$C$16,Tabelle1!$C$19,Tabelle1!$C$22,Tabelle1!$C$25)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>4.9249099999999997</c:v>
                 </c:pt>
-                <c:pt idx="1" formatCode="0.00000">
+                <c:pt idx="1" formatCode="000,000">
                   <c:v>6.8325800000000001</c:v>
                 </c:pt>
-                <c:pt idx="2" formatCode="0.00000">
+                <c:pt idx="2" formatCode="000,000">
                   <c:v>3.4630000000000001</c:v>
                 </c:pt>
-                <c:pt idx="3" formatCode="0.00000">
+                <c:pt idx="3" formatCode="000,000">
                   <c:v>2.4160599999999999</c:v>
                 </c:pt>
-                <c:pt idx="4" formatCode="0.00000">
+                <c:pt idx="4" formatCode="000,000">
                   <c:v>4.8210899999999999</c:v>
                 </c:pt>
-                <c:pt idx="5" formatCode="0.00000">
+                <c:pt idx="5" formatCode="000,000">
                   <c:v>1.4354499999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.2745599999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3252,8 +3354,8 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-408585952"/>
-        <c:axId val="-633256304"/>
+        <c:axId val="-1738646640"/>
+        <c:axId val="-1738643376"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredBarSeries>
@@ -3292,15 +3394,15 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>Tabelle1!$B$6:$B$22</c15:sqref>
+                          <c15:sqref>Tabelle1!$B$6:$B$25</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(Tabelle1!$B$7,Tabelle1!$B$10,Tabelle1!$B$13,Tabelle1!$B$16,Tabelle1!$B$19,Tabelle1!$B$22)</c15:sqref>
+                          <c15:sqref>(Tabelle1!$B$7,Tabelle1!$B$10,Tabelle1!$B$13,Tabelle1!$B$16,Tabelle1!$B$19,Tabelle1!$B$22,Tabelle1!$B$25)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:strCache>
-                      <c:ptCount val="6"/>
+                      <c:ptCount val="7"/>
                       <c:pt idx="0">
                         <c:v>1</c:v>
                       </c:pt>
@@ -3318,6 +3420,12 @@
                       </c:pt>
                       <c:pt idx="5">
                         <c:v>4.2</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>Dynamic</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>Dynamic</c:v>
                       </c:pt>
                     </c:strCache>
                   </c:strRef>
@@ -3341,16 +3449,16 @@
                         <c:v>0.21723400000000001</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>0</c:v>
+                        <c:v>3.3380874999999999</c:v>
                       </c:pt>
                       <c:pt idx="2">
                         <c:v>2.6963900000000001</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>0</c:v>
+                        <c:v>2.8530249999999997</c:v>
                       </c:pt>
                       <c:pt idx="4">
-                        <c:v>0</c:v>
+                        <c:v>2.0138775</c:v>
                       </c:pt>
                       <c:pt idx="5">
                         <c:v>0</c:v>
@@ -3366,7 +3474,7 @@
                 <c:order val="2"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Tabelle1!$E$5</c15:sqref>
@@ -3396,15 +3504,15 @@
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>Tabelle1!$B$6:$B$22</c15:sqref>
+                          <c15:sqref>Tabelle1!$B$6:$B$25</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(Tabelle1!$B$7,Tabelle1!$B$10,Tabelle1!$B$13,Tabelle1!$B$16,Tabelle1!$B$19,Tabelle1!$B$22)</c15:sqref>
+                          <c15:sqref>(Tabelle1!$B$7,Tabelle1!$B$10,Tabelle1!$B$13,Tabelle1!$B$16,Tabelle1!$B$19,Tabelle1!$B$22,Tabelle1!$B$25)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:strCache>
-                      <c:ptCount val="6"/>
+                      <c:ptCount val="7"/>
                       <c:pt idx="0">
                         <c:v>1</c:v>
                       </c:pt>
@@ -3422,6 +3530,12 @@
                       </c:pt>
                       <c:pt idx="5">
                         <c:v>4.2</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>Dynamic</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>Dynamic</c:v>
                       </c:pt>
                     </c:strCache>
                   </c:strRef>
@@ -3468,7 +3582,7 @@
         </c:extLst>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-408585952"/>
+        <c:axId val="-1738646640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3511,7 +3625,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-633256304"/>
+        <c:crossAx val="-1738643376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3519,7 +3633,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-633256304"/>
+        <c:axId val="-1738643376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3570,7 +3684,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-408585952"/>
+        <c:crossAx val="-1738646640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.5"/>
@@ -3758,13 +3872,13 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Tabelle1!$B$6:$B$22</c15:sqref>
+                    <c15:sqref>Tabelle1!$B$6:$B$25</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Tabelle1!$B$7,Tabelle1!$B$10,Tabelle1!$B$13,Tabelle1!$B$16,Tabelle1!$B$19,Tabelle1!$B$22)</c:f>
+              <c:f>(Tabelle1!$B$7,Tabelle1!$B$10,Tabelle1!$B$13,Tabelle1!$B$16,Tabelle1!$B$19,Tabelle1!$B$22,Tabelle1!$B$25)</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -3782,6 +3896,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>4.2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Dynamic</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3791,31 +3908,34 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Tabelle1!$D$6:$D$22</c15:sqref>
+                    <c15:sqref>Tabelle1!$D$6:$D$25</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Tabelle1!$D$7,Tabelle1!$D$10,Tabelle1!$D$13,Tabelle1!$D$16,Tabelle1!$D$19,Tabelle1!$D$22)</c:f>
+              <c:f>(Tabelle1!$D$7,Tabelle1!$D$10,Tabelle1!$D$13,Tabelle1!$D$16,Tabelle1!$D$19,Tabelle1!$D$22,Tabelle1!$D$25)</c:f>
               <c:numCache>
-                <c:formatCode>0.00000</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:formatCode>000,000</c:formatCode>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0.21723400000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>3.3380874999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>2.6963900000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>2.8530249999999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>2.0138775</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>2.2320550000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3831,8 +3951,8 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-408581056"/>
-        <c:axId val="-408587584"/>
+        <c:axId val="-1738642832"/>
+        <c:axId val="-1738644464"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredBarSeries>
@@ -3871,15 +3991,15 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>Tabelle1!$B$6:$B$22</c15:sqref>
+                          <c15:sqref>Tabelle1!$B$6:$B$25</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(Tabelle1!$B$7,Tabelle1!$B$10,Tabelle1!$B$13,Tabelle1!$B$16,Tabelle1!$B$19,Tabelle1!$B$22)</c15:sqref>
+                          <c15:sqref>(Tabelle1!$B$7,Tabelle1!$B$10,Tabelle1!$B$13,Tabelle1!$B$16,Tabelle1!$B$19,Tabelle1!$B$22,Tabelle1!$B$25)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:strCache>
-                      <c:ptCount val="6"/>
+                      <c:ptCount val="7"/>
                       <c:pt idx="0">
                         <c:v>1</c:v>
                       </c:pt>
@@ -3897,6 +4017,12 @@
                       </c:pt>
                       <c:pt idx="5">
                         <c:v>4.2</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>Dynamic</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>Dynamic</c:v>
                       </c:pt>
                     </c:strCache>
                   </c:strRef>
@@ -3945,7 +4071,7 @@
                 <c:order val="2"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Tabelle1!$E$5</c15:sqref>
@@ -3975,15 +4101,15 @@
                     <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:fullRef>
-                          <c15:sqref>Tabelle1!$B$6:$B$22</c15:sqref>
+                          <c15:sqref>Tabelle1!$B$6:$B$25</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(Tabelle1!$B$7,Tabelle1!$B$10,Tabelle1!$B$13,Tabelle1!$B$16,Tabelle1!$B$19,Tabelle1!$B$22)</c15:sqref>
+                          <c15:sqref>(Tabelle1!$B$7,Tabelle1!$B$10,Tabelle1!$B$13,Tabelle1!$B$16,Tabelle1!$B$19,Tabelle1!$B$22,Tabelle1!$B$25)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:strCache>
-                      <c:ptCount val="6"/>
+                      <c:ptCount val="7"/>
                       <c:pt idx="0">
                         <c:v>1</c:v>
                       </c:pt>
@@ -4001,6 +4127,12 @@
                       </c:pt>
                       <c:pt idx="5">
                         <c:v>4.2</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>Dynamic</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>Dynamic</c:v>
                       </c:pt>
                     </c:strCache>
                   </c:strRef>
@@ -4047,7 +4179,7 @@
         </c:extLst>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-408581056"/>
+        <c:axId val="-1738642832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4090,7 +4222,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-408587584"/>
+        <c:crossAx val="-1738644464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4098,7 +4230,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-408587584"/>
+        <c:axId val="-1738644464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4149,7 +4281,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-408581056"/>
+        <c:crossAx val="-1738642832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.25"/>
@@ -4337,13 +4469,13 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Tabelle1!$B$6:$B$22</c15:sqref>
+                    <c15:sqref>Tabelle1!$B$6:$B$25</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Tabelle1!$B$7,Tabelle1!$B$10,Tabelle1!$B$13,Tabelle1!$B$16,Tabelle1!$B$19,Tabelle1!$B$22)</c:f>
+              <c:f>(Tabelle1!$B$7,Tabelle1!$B$10,Tabelle1!$B$13,Tabelle1!$B$16,Tabelle1!$B$19,Tabelle1!$B$22,Tabelle1!$B$25)</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -4361,6 +4493,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>4.2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Dynamic</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4370,14 +4505,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Tabelle1!$C$6:$C$22</c15:sqref>
+                    <c15:sqref>Tabelle1!$C$6:$C$25</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Tabelle1!$C$7,Tabelle1!$C$10,Tabelle1!$C$13,Tabelle1!$C$16,Tabelle1!$C$19,Tabelle1!$C$22)</c:f>
+              <c:f>(Tabelle1!$C$7,Tabelle1!$C$10,Tabelle1!$C$13,Tabelle1!$C$16,Tabelle1!$C$19,Tabelle1!$C$22,Tabelle1!$C$25)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>4.9249099999999997</c:v>
                 </c:pt>
@@ -4395,6 +4530,9 @@
                 </c:pt>
                 <c:pt idx="5" formatCode="0.00000">
                   <c:v>1.4354499999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.2745599999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4429,13 +4567,13 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Tabelle1!$B$6:$B$22</c15:sqref>
+                    <c15:sqref>Tabelle1!$B$6:$B$25</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Tabelle1!$B$7,Tabelle1!$B$10,Tabelle1!$B$13,Tabelle1!$B$16,Tabelle1!$B$19,Tabelle1!$B$22)</c:f>
+              <c:f>(Tabelle1!$B$7,Tabelle1!$B$10,Tabelle1!$B$13,Tabelle1!$B$16,Tabelle1!$B$19,Tabelle1!$B$22,Tabelle1!$B$25)</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -4453,6 +4591,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>4.2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Dynamic</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4462,31 +4603,34 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Tabelle1!$D$6:$D$22</c15:sqref>
+                    <c15:sqref>Tabelle1!$D$6:$D$25</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Tabelle1!$D$7,Tabelle1!$D$10,Tabelle1!$D$13,Tabelle1!$D$16,Tabelle1!$D$19,Tabelle1!$D$22)</c:f>
+              <c:f>(Tabelle1!$D$7,Tabelle1!$D$10,Tabelle1!$D$13,Tabelle1!$D$16,Tabelle1!$D$19,Tabelle1!$D$22,Tabelle1!$D$25)</c:f>
               <c:numCache>
                 <c:formatCode>0.00000</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0.21723400000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>3.3380874999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>2.6963900000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>2.8530249999999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>2.0138775</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>2.2320550000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4521,13 +4665,13 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Tabelle1!$B$6:$B$22</c15:sqref>
+                    <c15:sqref>Tabelle1!$B$6:$B$25</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Tabelle1!$B$7,Tabelle1!$B$10,Tabelle1!$B$13,Tabelle1!$B$16,Tabelle1!$B$19,Tabelle1!$B$22)</c:f>
+              <c:f>(Tabelle1!$B$7,Tabelle1!$B$10,Tabelle1!$B$13,Tabelle1!$B$16,Tabelle1!$B$19,Tabelle1!$B$22,Tabelle1!$B$25)</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -4545,6 +4689,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>4.2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Dynamic</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4554,14 +4701,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Tabelle1!$E$6:$E$22</c15:sqref>
+                    <c15:sqref>Tabelle1!$E$6:$E$25</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Tabelle1!$E$7,Tabelle1!$E$10,Tabelle1!$E$13,Tabelle1!$E$16,Tabelle1!$E$19,Tabelle1!$E$22)</c:f>
+              <c:f>(Tabelle1!$E$7,Tabelle1!$E$10,Tabelle1!$E$13,Tabelle1!$E$16,Tabelle1!$E$19,Tabelle1!$E$22,Tabelle1!$E$25)</c:f>
               <c:numCache>
-                <c:formatCode>0.00000</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:formatCode>000,000</c:formatCode>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>8.5662699999999994E-2</c:v>
                 </c:pt>
@@ -4579,6 +4726,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.75661400000000001</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>0.82827700000000004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4594,11 +4744,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-589329200"/>
-        <c:axId val="-514878096"/>
+        <c:axId val="-1738641200"/>
+        <c:axId val="-1738652080"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-589329200"/>
+        <c:axId val="-1738641200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4641,7 +4791,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-514878096"/>
+        <c:crossAx val="-1738652080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4649,7 +4799,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-514878096"/>
+        <c:axId val="-1738652080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4700,7 +4850,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-589329200"/>
+        <c:crossAx val="-1738641200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9635,13 +9785,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AA68" sqref="AA68"/>
+    <sheetView tabSelected="1" topLeftCell="Q79" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
         <v>0</v>
       </c>
@@ -9652,7 +9802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>8</v>
       </c>
@@ -9667,7 +9817,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>9</v>
       </c>
@@ -9681,7 +9831,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B6" s="1">
         <v>1</v>
       </c>
@@ -9698,7 +9848,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B7" s="1">
         <v>1</v>
       </c>
@@ -9715,22 +9865,23 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B8" s="1"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="3"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B9" s="1">
         <v>2</v>
       </c>
       <c r="C9" s="2">
         <v>0.43307000000000001</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>12</v>
+      <c r="D9" s="8">
+        <f>(0.57981+0.57683+0.581912+0.578102)/4</f>
+        <v>0.57916349999999994</v>
       </c>
       <c r="E9" s="2">
         <v>0.77977624999999995</v>
@@ -9739,15 +9890,16 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B10" s="1">
         <v>2</v>
       </c>
       <c r="C10" s="2">
         <v>6.8325800000000001</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>12</v>
+      <c r="D10" s="8">
+        <f>(3.34028+3.34108+3.33607+3.33492)/4</f>
+        <v>3.3380874999999999</v>
       </c>
       <c r="E10" s="2">
         <v>2.7210800000000002</v>
@@ -9756,14 +9908,14 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B11" s="1"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="3"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B12" s="1">
         <v>3</v>
       </c>
@@ -9780,7 +9932,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B13" s="1">
         <v>3</v>
       </c>
@@ -9797,14 +9949,14 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B14" s="1"/>
       <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
+      <c r="D14" s="8"/>
       <c r="E14" s="2"/>
       <c r="F14" s="3"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B15" s="1">
         <v>4</v>
       </c>
@@ -9812,8 +9964,9 @@
         <f>(1.01107+1.0242+1.0322+1.01348)/4</f>
         <v>1.0202374999999999</v>
       </c>
-      <c r="D15" s="4" t="s">
-        <v>12</v>
+      <c r="D15" s="8">
+        <f>(0.661035+0.660433+0.660824+0.657562)/4</f>
+        <v>0.65996350000000004</v>
       </c>
       <c r="E15" s="2">
         <f>(1.10844+1.1032+1.11739)/3</f>
@@ -9826,15 +9979,16 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B16" s="1">
         <v>4</v>
       </c>
       <c r="C16" s="2">
         <v>2.4160599999999999</v>
       </c>
-      <c r="D16" s="4" t="s">
-        <v>12</v>
+      <c r="D16" s="8">
+        <f>(2.85531+2.85449+2.84999+2.85231)/4</f>
+        <v>2.8530249999999997</v>
       </c>
       <c r="E16" s="2">
         <v>1.7616400000000001</v>
@@ -9843,22 +9997,23 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B17" s="1"/>
       <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
+      <c r="D17" s="8"/>
       <c r="E17" s="2"/>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B18" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C18" s="2">
         <v>0.5261922</v>
       </c>
-      <c r="D18" s="4" t="s">
-        <v>12</v>
+      <c r="D18" s="8">
+        <f>(0.899913+0.899776+0.895833+0.90112)/4</f>
+        <v>0.89916050000000003</v>
       </c>
       <c r="E18" s="2">
         <f>(0.850354+0.842024+0.840035)/3</f>
@@ -9871,15 +10026,16 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B19" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C19" s="2">
         <v>4.8210899999999999</v>
       </c>
-      <c r="D19" s="4" t="s">
-        <v>12</v>
+      <c r="D19" s="8">
+        <f>(2.01356+2.01146+2.01594+2.01455)/4</f>
+        <v>2.0138775</v>
       </c>
       <c r="E19" s="2">
         <v>2.47004</v>
@@ -9888,13 +10044,13 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B20" s="1"/>
       <c r="C20" s="2"/>
       <c r="D20" s="4"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B21" s="5" t="s">
         <v>16</v>
       </c>
@@ -9916,7 +10072,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B22" s="5" t="s">
         <v>16</v>
       </c>
@@ -9933,22 +10089,56 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B23" s="1"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="1"/>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B24" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24">
+        <f>(0.809555+0.799533+0.817558+0.817221)/4</f>
+        <v>0.81096674999999996</v>
+      </c>
+      <c r="D24">
+        <f>(0.917866+0.92266+0.918336+0.916579)/4</f>
+        <v>0.91886025000000005</v>
+      </c>
+      <c r="E24">
+        <f>(2.9264+2.94111+2.91605+2.91507)/4</f>
+        <v>2.9246574999999999</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="1"/>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B25" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25">
+        <f>(3.2118+3.39012+3.24621+3.25011)/4</f>
+        <v>3.2745599999999997</v>
+      </c>
+      <c r="D25">
+        <f>(2.2326+2.23164+2.2322+2.23178)/4</f>
+        <v>2.2320550000000003</v>
+      </c>
+      <c r="E25">
+        <f>(0.826045+0.82276+0.831475+0.832828)/4</f>
+        <v>0.82827700000000004</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B26" s="1"/>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B27" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
collected Data and updated kernel exel file
</commit_message>
<xml_diff>
--- a/Output/Kernel vergleich.xlsx
+++ b/Output/Kernel vergleich.xlsx
@@ -290,7 +290,224 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr sz="1400">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+              </a:rPr>
+              <a:t>Barts Runtime in S</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$E$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Barts</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ff0000"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:dLbls>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Tabelle1!$B$6;Tabelle1!$B$9;Tabelle1!$B$12;Tabelle1!$B$15;Tabelle1!$B$18;Tabelle1!$B$21;Tabelle1!$B$24</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Dynamic</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$E$6;Tabelle1!$E$9;Tabelle1!$E$12;Tabelle1!$E$15;Tabelle1!$E$18;Tabelle1!$E$21;Tabelle1!$E$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>19.013</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.77977625</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.15306</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.10967666666667</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.844137666666667</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.954555</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.3757225</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="97097982"/>
+        <c:axId val="49512146"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="97097982"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="9360">
+            <a:solidFill>
+              <a:srgbClr val="d9d9d9"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="49512146"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="49512146"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="20"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9360">
+              <a:solidFill>
+                <a:srgbClr val="d9d9d9"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="6480">
+            <a:solidFill>
+              <a:srgbClr val="5b9bd5"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="97097982"/>
+        <c:crosses val="autoZero"/>
+        <c:majorUnit val="1"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="9360">
+      <a:solidFill>
+        <a:srgbClr val="d9d9d9"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -406,7 +623,7 @@
                   <c:v>1.1054575</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.81096675</c:v>
+                  <c:v>0.6401595</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -414,11 +631,11 @@
         </c:ser>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="86983862"/>
-        <c:axId val="18272950"/>
+        <c:axId val="18197117"/>
+        <c:axId val="92343503"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="86983862"/>
+        <c:axId val="18197117"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -435,14 +652,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="18272950"/>
+        <c:crossAx val="92343503"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="18272950"/>
+        <c:axId val="92343503"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -466,7 +683,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="86983862"/>
+        <c:crossAx val="18197117"/>
         <c:crosses val="autoZero"/>
         <c:majorUnit val="0.1"/>
       </c:valAx>
@@ -503,7 +720,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -619,7 +836,7 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.91886025</c:v>
+                  <c:v>0.81985075</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -627,11 +844,11 @@
         </c:ser>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="49099790"/>
-        <c:axId val="90430404"/>
+        <c:axId val="34091406"/>
+        <c:axId val="95131457"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="49099790"/>
+        <c:axId val="34091406"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -648,14 +865,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="90430404"/>
+        <c:crossAx val="95131457"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="90430404"/>
+        <c:axId val="95131457"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -679,7 +896,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="49099790"/>
+        <c:crossAx val="34091406"/>
         <c:crosses val="autoZero"/>
         <c:majorUnit val="1"/>
       </c:valAx>
@@ -716,7 +933,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart20.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -832,7 +1049,7 @@
                   <c:v>1.1054575</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.81096675</c:v>
+                  <c:v>0.6401595</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -922,7 +1139,7 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.91886025</c:v>
+                  <c:v>0.81985075</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1020,11 +1237,11 @@
         </c:ser>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="61038136"/>
-        <c:axId val="36881725"/>
+        <c:axId val="56214695"/>
+        <c:axId val="23418383"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="61038136"/>
+        <c:axId val="56214695"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1041,14 +1258,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="36881725"/>
+        <c:crossAx val="23418383"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="36881725"/>
+        <c:axId val="23418383"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1072,7 +1289,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="61038136"/>
+        <c:crossAx val="56214695"/>
         <c:crosses val="autoZero"/>
         <c:majorUnit val="1"/>
       </c:valAx>
@@ -1109,7 +1326,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart21.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -1233,11 +1450,11 @@
         </c:ser>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="34443820"/>
-        <c:axId val="77046351"/>
+        <c:axId val="68858129"/>
+        <c:axId val="51617708"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="34443820"/>
+        <c:axId val="68858129"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1254,14 +1471,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="77046351"/>
+        <c:crossAx val="51617708"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="77046351"/>
+        <c:axId val="51617708"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1285,7 +1502,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="34443820"/>
+        <c:crossAx val="68858129"/>
         <c:crosses val="autoZero"/>
         <c:majorUnit val="0.25"/>
       </c:valAx>
@@ -1322,7 +1539,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart22.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -1438,7 +1655,7 @@
                   <c:v>1.43545</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.27456</c:v>
+                  <c:v>3.8240875</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1446,11 +1663,11 @@
         </c:ser>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="92567692"/>
-        <c:axId val="6849041"/>
+        <c:axId val="12254272"/>
+        <c:axId val="47271633"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="92567692"/>
+        <c:axId val="12254272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1467,14 +1684,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="6849041"/>
+        <c:crossAx val="47271633"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="6849041"/>
+        <c:axId val="47271633"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1498,7 +1715,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="92567692"/>
+        <c:crossAx val="12254272"/>
         <c:crosses val="autoZero"/>
         <c:majorUnit val="0.5"/>
       </c:valAx>
@@ -1535,7 +1752,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart23.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -1651,7 +1868,7 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.232055</c:v>
+                  <c:v>2.2293775</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1659,11 +1876,11 @@
         </c:ser>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="26366273"/>
-        <c:axId val="77275442"/>
+        <c:axId val="44399842"/>
+        <c:axId val="66845863"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="26366273"/>
+        <c:axId val="44399842"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1680,14 +1897,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="77275442"/>
+        <c:crossAx val="66845863"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="77275442"/>
+        <c:axId val="66845863"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1711,7 +1928,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="26366273"/>
+        <c:crossAx val="44399842"/>
         <c:crosses val="autoZero"/>
         <c:majorUnit val="0.25"/>
       </c:valAx>
@@ -1748,7 +1965,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart24.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -1864,7 +2081,7 @@
                   <c:v>1.43545</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.27456</c:v>
+                  <c:v>3.8240875</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1954,7 +2171,7 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.232055</c:v>
+                  <c:v>2.2293775</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2052,11 +2269,11 @@
         </c:ser>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="60696922"/>
-        <c:axId val="42311140"/>
+        <c:axId val="86129348"/>
+        <c:axId val="97197549"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="60696922"/>
+        <c:axId val="86129348"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2073,14 +2290,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="42311140"/>
+        <c:crossAx val="97197549"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="42311140"/>
+        <c:axId val="97197549"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2104,225 +2321,8 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="60696922"/>
+        <c:crossAx val="86129348"/>
         <c:crosses val="autoZero"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln w="9360">
-      <a:solidFill>
-        <a:srgbClr val="d9d9d9"/>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr sz="1400">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri"/>
-              </a:rPr>
-              <a:t>Barts Runtime in S</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-    </c:title>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Tabelle1!$E$5</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Barts</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="ff0000"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:dLbls>
-            <c:dLblPos val="ctr"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>Tabelle1!$B$6;Tabelle1!$B$9;Tabelle1!$B$12;Tabelle1!$B$15;Tabelle1!$B$18;Tabelle1!$B$21;Tabelle1!$B$24</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4.1</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4.2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Dynamic</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Tabelle1!$E$6;Tabelle1!$E$9;Tabelle1!$E$12;Tabelle1!$E$15;Tabelle1!$E$18;Tabelle1!$E$21;Tabelle1!$E$24</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>19.013</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.77977625</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.15306</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.10967666666667</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.844137666666667</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.954555</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2.3757225</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="6004125"/>
-        <c:axId val="44581481"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="6004125"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="9360">
-            <a:solidFill>
-              <a:srgbClr val="d9d9d9"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-        </c:spPr>
-        <c:crossAx val="44581481"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="44581481"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:max val="20"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9360">
-              <a:solidFill>
-                <a:srgbClr val="d9d9d9"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="6480">
-            <a:solidFill>
-              <a:srgbClr val="5b9bd5"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-        </c:spPr>
-        <c:crossAx val="6004125"/>
-        <c:crosses val="autoZero"/>
-        <c:majorUnit val="1"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -2610,7 +2610,7 @@
   <dimension ref="A3:G28"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D28" activeCellId="0" sqref="D28"/>
+      <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2927,12 +2927,12 @@
         <v>18</v>
       </c>
       <c r="C24" s="0" t="n">
-        <f aca="false">(0.809555+0.799533+0.817558+0.817221)/4</f>
-        <v>0.81096675</v>
+        <f aca="false">(0.60382+0.61476+0.604918+0.73714)/4</f>
+        <v>0.6401595</v>
       </c>
       <c r="D24" s="0" t="n">
-        <f aca="false">(0.917866+0.92266+0.918336+0.916579)/4</f>
-        <v>0.91886025</v>
+        <f aca="false">(0.818113+0.823809+0.819304+0.818177)/4</f>
+        <v>0.81985075</v>
       </c>
       <c r="E24" s="0" t="n">
         <f aca="false">(2.56391+2.31429+2.30321+2.32148)/4</f>
@@ -2947,12 +2947,12 @@
         <v>18</v>
       </c>
       <c r="C25" s="0" t="n">
-        <f aca="false">(3.2118+3.39012+3.24621+3.25011)/4</f>
-        <v>3.27456</v>
+        <f aca="false">(3.77988+3.71921+3.76059+4.03667 )/4</f>
+        <v>3.8240875</v>
       </c>
       <c r="D25" s="0" t="n">
-        <f aca="false">(2.2326+2.23164+2.2322+2.23178)/4</f>
-        <v>2.232055</v>
+        <f aca="false">(2.22981+2.22904+2.22949+2.22917)/4</f>
+        <v>2.2293775</v>
       </c>
       <c r="E25" s="0" t="n">
         <f aca="false">(0.722009+0.794159+0.795563 +0.790121 )/4</f>
@@ -2970,6 +2970,14 @@
       <c r="B27" s="3" t="s">
         <v>19</v>
       </c>
+      <c r="C27" s="0" t="n">
+        <f aca="false">(0.38893+0.428742+0.411657+0.411178)/4</f>
+        <v>0.41012675</v>
+      </c>
+      <c r="D27" s="0" t="n">
+        <f aca="false">(0.556837+0.555766+0.559186+0.553763)/4</f>
+        <v>0.556388</v>
+      </c>
       <c r="E27" s="0" t="n">
         <f aca="false">(0.770456+0.80318+0.798453+0.802236)/4</f>
         <v>0.79358125</v>
@@ -2981,6 +2989,14 @@
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="9" t="s">
         <v>19</v>
+      </c>
+      <c r="C28" s="0" t="n">
+        <f aca="false">(5.94859+5.16703+5.60233+5.71391)/4</f>
+        <v>5.607965</v>
+      </c>
+      <c r="D28" s="0" t="n">
+        <f aca="false">(3.48563+3.48459+3.48599+3.48248)/4</f>
+        <v>3.4846725</v>
       </c>
       <c r="E28" s="10" t="n">
         <f aca="false">(2.78492+2.71566+2.71721+2.73853)/4</f>

</xml_diff>

<commit_message>
Corrected error in Exel file
</commit_message>
<xml_diff>
--- a/Output/Kernel vergleich.xlsx
+++ b/Output/Kernel vergleich.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="29">
   <si>
     <t>AMD</t>
   </si>
@@ -150,7 +150,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -159,12 +159,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -450,11 +446,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-160210768"/>
-        <c:axId val="-160223824"/>
+        <c:axId val="1465942768"/>
+        <c:axId val="1465945488"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-160210768"/>
+        <c:axId val="1465942768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -472,7 +468,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="-160223824"/>
+        <c:crossAx val="1465945488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -480,7 +476,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-160223824"/>
+        <c:axId val="1465945488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="20"/>
@@ -509,7 +505,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="-160210768"/>
+        <c:crossAx val="1465942768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -654,7 +650,7 @@
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Tabelle1!$B$9,Tabelle1!$B$12,Tabelle1!$B$15,Tabelle1!$B$18,Tabelle1!$B$27,Tabelle1!$B$30,Tabelle1!$B$33)</c:f>
+              <c:f>(Tabelle1!$B$9,Tabelle1!$B$12,Tabelle1!$B$15,Tabelle1!$B$21,Tabelle1!$B$27,Tabelle1!$B$30,Tabelle1!$B$33)</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -667,7 +663,7 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>4.1</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>Dynamic</c:v>
@@ -690,7 +686,7 @@
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Tabelle1!$G$9,Tabelle1!$G$12,Tabelle1!$G$15,Tabelle1!$G$18,Tabelle1!$G$27,Tabelle1!$G$30,Tabelle1!$G$33)</c:f>
+              <c:f>(Tabelle1!$G$9,Tabelle1!$G$12,Tabelle1!$G$15,Tabelle1!$G$21,Tabelle1!$G$27,Tabelle1!$G$30,Tabelle1!$G$33)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -729,8 +725,8 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-96056496"/>
-        <c:axId val="-96055408"/>
+        <c:axId val="1516394720"/>
+        <c:axId val="1516399072"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredBarSeries>
@@ -772,7 +768,7 @@
                           <c15:sqref>Tabelle1!$B$6:$B$33</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(Tabelle1!$B$9,Tabelle1!$B$12,Tabelle1!$B$15,Tabelle1!$B$18,Tabelle1!$B$27,Tabelle1!$B$30,Tabelle1!$B$33)</c15:sqref>
+                          <c15:sqref>(Tabelle1!$B$9,Tabelle1!$B$12,Tabelle1!$B$15,Tabelle1!$B$21,Tabelle1!$B$27,Tabelle1!$B$30,Tabelle1!$B$33)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -788,7 +784,7 @@
                         <c:v>3</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>4</c:v>
+                        <c:v>4.1</c:v>
                       </c:pt>
                       <c:pt idx="4">
                         <c:v>Dynamic</c:v>
@@ -810,7 +806,7 @@
                           <c15:sqref>Tabelle1!$C$6:$C$33</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(Tabelle1!$C$9,Tabelle1!$C$12,Tabelle1!$C$15,Tabelle1!$C$18,Tabelle1!$C$27,Tabelle1!$C$30,Tabelle1!$C$33)</c15:sqref>
+                          <c15:sqref>(Tabelle1!$C$9,Tabelle1!$C$12,Tabelle1!$C$15,Tabelle1!$C$21,Tabelle1!$C$27,Tabelle1!$C$30,Tabelle1!$C$33)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -827,13 +823,16 @@
                         <c:v>3.4630000000000001</c:v>
                       </c:pt>
                       <c:pt idx="3" formatCode="0.00000">
-                        <c:v>2.4160599999999999</c:v>
+                        <c:v>4.8210899999999999</c:v>
                       </c:pt>
                       <c:pt idx="4" formatCode="0.00000">
                         <c:v>3.8240875000000001</c:v>
                       </c:pt>
                       <c:pt idx="5" formatCode="0.00000">
                         <c:v>5.6079650000000001</c:v>
+                      </c:pt>
+                      <c:pt idx="6" formatCode="0.00000">
+                        <c:v>0</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -846,7 +845,7 @@
                 <c:order val="1"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Tabelle1!$D$5</c15:sqref>
@@ -879,7 +878,7 @@
                           <c15:sqref>Tabelle1!$B$6:$B$33</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(Tabelle1!$B$9,Tabelle1!$B$12,Tabelle1!$B$15,Tabelle1!$B$18,Tabelle1!$B$27,Tabelle1!$B$30,Tabelle1!$B$33)</c15:sqref>
+                          <c15:sqref>(Tabelle1!$B$9,Tabelle1!$B$12,Tabelle1!$B$15,Tabelle1!$B$21,Tabelle1!$B$27,Tabelle1!$B$30,Tabelle1!$B$33)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -895,7 +894,7 @@
                         <c:v>3</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>4</c:v>
+                        <c:v>4.1</c:v>
                       </c:pt>
                       <c:pt idx="4">
                         <c:v>Dynamic</c:v>
@@ -917,7 +916,7 @@
                           <c15:sqref>Tabelle1!$D$6:$D$33</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(Tabelle1!$D$9,Tabelle1!$D$12,Tabelle1!$D$15,Tabelle1!$D$18,Tabelle1!$D$27,Tabelle1!$D$30,Tabelle1!$D$33)</c15:sqref>
+                          <c15:sqref>(Tabelle1!$D$9,Tabelle1!$D$12,Tabelle1!$D$15,Tabelle1!$D$21,Tabelle1!$D$27,Tabelle1!$D$30,Tabelle1!$D$33)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -934,13 +933,16 @@
                         <c:v>2.6963900000000001</c:v>
                       </c:pt>
                       <c:pt idx="3" formatCode="0.00000">
-                        <c:v>2.8530249999999997</c:v>
+                        <c:v>2.0138775</c:v>
                       </c:pt>
                       <c:pt idx="4" formatCode="0.00000">
                         <c:v>2.2293775</c:v>
                       </c:pt>
                       <c:pt idx="5" formatCode="0.00000">
                         <c:v>3.4846724999999994</c:v>
+                      </c:pt>
+                      <c:pt idx="6" formatCode="0.00000">
+                        <c:v>0</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -953,7 +955,7 @@
                 <c:order val="2"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Tabelle1!$E$5</c15:sqref>
@@ -986,7 +988,7 @@
                           <c15:sqref>Tabelle1!$B$6:$B$33</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(Tabelle1!$B$9,Tabelle1!$B$12,Tabelle1!$B$15,Tabelle1!$B$18,Tabelle1!$B$27,Tabelle1!$B$30,Tabelle1!$B$33)</c15:sqref>
+                          <c15:sqref>(Tabelle1!$B$9,Tabelle1!$B$12,Tabelle1!$B$15,Tabelle1!$B$21,Tabelle1!$B$27,Tabelle1!$B$30,Tabelle1!$B$33)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1002,7 +1004,7 @@
                         <c:v>3</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>4</c:v>
+                        <c:v>4.1</c:v>
                       </c:pt>
                       <c:pt idx="4">
                         <c:v>Dynamic</c:v>
@@ -1024,7 +1026,7 @@
                           <c15:sqref>Tabelle1!$E$6:$E$33</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(Tabelle1!$E$9,Tabelle1!$E$12,Tabelle1!$E$15,Tabelle1!$E$18,Tabelle1!$E$27,Tabelle1!$E$30,Tabelle1!$E$33)</c15:sqref>
+                          <c15:sqref>(Tabelle1!$E$9,Tabelle1!$E$12,Tabelle1!$E$15,Tabelle1!$E$21,Tabelle1!$E$27,Tabelle1!$E$30,Tabelle1!$E$33)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1041,13 +1043,16 @@
                         <c:v>0.76924999999999999</c:v>
                       </c:pt>
                       <c:pt idx="3" formatCode="0.00000">
-                        <c:v>1.7616400000000001</c:v>
+                        <c:v>2.47004</c:v>
                       </c:pt>
                       <c:pt idx="4" formatCode="0.00000">
                         <c:v>0.77546300000000001</c:v>
                       </c:pt>
                       <c:pt idx="5" formatCode="0.00000">
                         <c:v>2.7390800000000004</c:v>
+                      </c:pt>
+                      <c:pt idx="6" formatCode="0.00000">
+                        <c:v>0</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1060,7 +1065,7 @@
                 <c:order val="3"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Tabelle1!$F$5</c15:sqref>
@@ -1093,7 +1098,7 @@
                           <c15:sqref>Tabelle1!$B$6:$B$33</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(Tabelle1!$B$9,Tabelle1!$B$12,Tabelle1!$B$15,Tabelle1!$B$18,Tabelle1!$B$27,Tabelle1!$B$30,Tabelle1!$B$33)</c15:sqref>
+                          <c15:sqref>(Tabelle1!$B$9,Tabelle1!$B$12,Tabelle1!$B$15,Tabelle1!$B$21,Tabelle1!$B$27,Tabelle1!$B$30,Tabelle1!$B$33)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1109,7 +1114,7 @@
                         <c:v>3</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>4</c:v>
+                        <c:v>4.1</c:v>
                       </c:pt>
                       <c:pt idx="4">
                         <c:v>Dynamic</c:v>
@@ -1131,7 +1136,7 @@
                           <c15:sqref>Tabelle1!$F$6:$F$33</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(Tabelle1!$F$9,Tabelle1!$F$12,Tabelle1!$F$15,Tabelle1!$F$18,Tabelle1!$F$27,Tabelle1!$F$30,Tabelle1!$F$33)</c15:sqref>
+                          <c15:sqref>(Tabelle1!$F$9,Tabelle1!$F$12,Tabelle1!$F$15,Tabelle1!$F$21,Tabelle1!$F$27,Tabelle1!$F$30,Tabelle1!$F$33)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1168,7 +1173,7 @@
         </c:extLst>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-96056496"/>
+        <c:axId val="1516394720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1211,7 +1216,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-96055408"/>
+        <c:crossAx val="1516399072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1219,7 +1224,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-96055408"/>
+        <c:axId val="1516399072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1270,7 +1275,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-96056496"/>
+        <c:crossAx val="1516394720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1433,7 +1438,7 @@
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Tabelle1!$B$8,Tabelle1!$B$11,Tabelle1!$B$14,Tabelle1!$B$17,Tabelle1!$B$26,Tabelle1!$B$29,Tabelle1!$B$32)</c:f>
+              <c:f>(Tabelle1!$B$8,Tabelle1!$B$11,Tabelle1!$B$14,Tabelle1!$B$20,Tabelle1!$B$26,Tabelle1!$B$29,Tabelle1!$B$32)</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -1446,7 +1451,7 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>4.1</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>Dynamic</c:v>
@@ -1469,7 +1474,7 @@
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Tabelle1!$F$8,Tabelle1!$F$11,Tabelle1!$F$14,Tabelle1!$F$17,Tabelle1!$F$26,Tabelle1!$F$29,Tabelle1!$F$32)</c:f>
+              <c:f>(Tabelle1!$F$8,Tabelle1!$F$11,Tabelle1!$F$14,Tabelle1!$F$20,Tabelle1!$F$26,Tabelle1!$F$29,Tabelle1!$F$32)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1508,8 +1513,8 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-94638256"/>
-        <c:axId val="-94643152"/>
+        <c:axId val="1516397440"/>
+        <c:axId val="1516394176"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredBarSeries>
@@ -1551,7 +1556,7 @@
                           <c15:sqref>Tabelle1!$B$6:$B$33</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(Tabelle1!$B$8,Tabelle1!$B$11,Tabelle1!$B$14,Tabelle1!$B$17,Tabelle1!$B$26,Tabelle1!$B$29,Tabelle1!$B$32)</c15:sqref>
+                          <c15:sqref>(Tabelle1!$B$8,Tabelle1!$B$11,Tabelle1!$B$14,Tabelle1!$B$20,Tabelle1!$B$26,Tabelle1!$B$29,Tabelle1!$B$32)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1567,7 +1572,7 @@
                         <c:v>3</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>4</c:v>
+                        <c:v>4.1</c:v>
                       </c:pt>
                       <c:pt idx="4">
                         <c:v>Dynamic</c:v>
@@ -1589,7 +1594,7 @@
                           <c15:sqref>Tabelle1!$C$6:$C$33</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(Tabelle1!$C$8,Tabelle1!$C$11,Tabelle1!$C$14,Tabelle1!$C$17,Tabelle1!$C$26,Tabelle1!$C$29,Tabelle1!$C$32)</c15:sqref>
+                          <c15:sqref>(Tabelle1!$C$8,Tabelle1!$C$11,Tabelle1!$C$14,Tabelle1!$C$20,Tabelle1!$C$26,Tabelle1!$C$29,Tabelle1!$C$32)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1606,13 +1611,16 @@
                         <c:v>0.69523500000000005</c:v>
                       </c:pt>
                       <c:pt idx="3" formatCode="0.00000">
-                        <c:v>1.0202374999999999</c:v>
+                        <c:v>0.5261922</c:v>
                       </c:pt>
                       <c:pt idx="4" formatCode="0.00000">
                         <c:v>0.64015949999999999</c:v>
                       </c:pt>
                       <c:pt idx="5" formatCode="0.00000">
                         <c:v>0.41012674999999998</c:v>
+                      </c:pt>
+                      <c:pt idx="6" formatCode="0.00000">
+                        <c:v>0</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1625,7 +1633,7 @@
                 <c:order val="1"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Tabelle1!$D$5</c15:sqref>
@@ -1658,7 +1666,7 @@
                           <c15:sqref>Tabelle1!$B$6:$B$33</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(Tabelle1!$B$8,Tabelle1!$B$11,Tabelle1!$B$14,Tabelle1!$B$17,Tabelle1!$B$26,Tabelle1!$B$29,Tabelle1!$B$32)</c15:sqref>
+                          <c15:sqref>(Tabelle1!$B$8,Tabelle1!$B$11,Tabelle1!$B$14,Tabelle1!$B$20,Tabelle1!$B$26,Tabelle1!$B$29,Tabelle1!$B$32)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1674,7 +1682,7 @@
                         <c:v>3</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>4</c:v>
+                        <c:v>4.1</c:v>
                       </c:pt>
                       <c:pt idx="4">
                         <c:v>Dynamic</c:v>
@@ -1696,7 +1704,7 @@
                           <c15:sqref>Tabelle1!$D$6:$D$33</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(Tabelle1!$D$8,Tabelle1!$D$11,Tabelle1!$D$14,Tabelle1!$D$17,Tabelle1!$D$26,Tabelle1!$D$29,Tabelle1!$D$32)</c15:sqref>
+                          <c15:sqref>(Tabelle1!$D$8,Tabelle1!$D$11,Tabelle1!$D$14,Tabelle1!$D$20,Tabelle1!$D$26,Tabelle1!$D$29,Tabelle1!$D$32)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1713,13 +1721,16 @@
                         <c:v>0.69224300000000005</c:v>
                       </c:pt>
                       <c:pt idx="3" formatCode="0.00000">
-                        <c:v>0.65996350000000004</c:v>
+                        <c:v>0.89916050000000003</c:v>
                       </c:pt>
                       <c:pt idx="4" formatCode="0.00000">
                         <c:v>0.81985074999999996</c:v>
                       </c:pt>
                       <c:pt idx="5" formatCode="0.00000">
                         <c:v>0.55638799999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="6" formatCode="0.00000">
+                        <c:v>0</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1732,7 +1743,7 @@
                 <c:order val="2"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Tabelle1!$E$5</c15:sqref>
@@ -1765,7 +1776,7 @@
                           <c15:sqref>Tabelle1!$B$6:$B$33</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(Tabelle1!$B$8,Tabelle1!$B$11,Tabelle1!$B$14,Tabelle1!$B$17,Tabelle1!$B$26,Tabelle1!$B$29,Tabelle1!$B$32)</c15:sqref>
+                          <c15:sqref>(Tabelle1!$B$8,Tabelle1!$B$11,Tabelle1!$B$14,Tabelle1!$B$20,Tabelle1!$B$26,Tabelle1!$B$29,Tabelle1!$B$32)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1781,7 +1792,7 @@
                         <c:v>3</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>4</c:v>
+                        <c:v>4.1</c:v>
                       </c:pt>
                       <c:pt idx="4">
                         <c:v>Dynamic</c:v>
@@ -1803,7 +1814,7 @@
                           <c15:sqref>Tabelle1!$E$6:$E$33</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(Tabelle1!$E$8,Tabelle1!$E$11,Tabelle1!$E$14,Tabelle1!$E$17,Tabelle1!$E$26,Tabelle1!$E$29,Tabelle1!$E$32)</c15:sqref>
+                          <c15:sqref>(Tabelle1!$E$8,Tabelle1!$E$11,Tabelle1!$E$14,Tabelle1!$E$20,Tabelle1!$E$26,Tabelle1!$E$29,Tabelle1!$E$32)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1820,13 +1831,16 @@
                         <c:v>2.15306</c:v>
                       </c:pt>
                       <c:pt idx="3" formatCode="0.00000">
-                        <c:v>1.1096766666666669</c:v>
+                        <c:v>0.84413766666666668</c:v>
                       </c:pt>
                       <c:pt idx="4" formatCode="0.00000">
                         <c:v>2.3757225000000002</c:v>
                       </c:pt>
                       <c:pt idx="5" formatCode="0.00000">
                         <c:v>0.7935812499999999</c:v>
+                      </c:pt>
+                      <c:pt idx="6" formatCode="0.00000">
+                        <c:v>0</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1839,7 +1853,7 @@
                 <c:order val="4"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Tabelle1!$G$5</c15:sqref>
@@ -1872,7 +1886,7 @@
                           <c15:sqref>Tabelle1!$B$6:$B$33</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(Tabelle1!$B$8,Tabelle1!$B$11,Tabelle1!$B$14,Tabelle1!$B$17,Tabelle1!$B$26,Tabelle1!$B$29,Tabelle1!$B$32)</c15:sqref>
+                          <c15:sqref>(Tabelle1!$B$8,Tabelle1!$B$11,Tabelle1!$B$14,Tabelle1!$B$20,Tabelle1!$B$26,Tabelle1!$B$29,Tabelle1!$B$32)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1888,7 +1902,7 @@
                         <c:v>3</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>4</c:v>
+                        <c:v>4.1</c:v>
                       </c:pt>
                       <c:pt idx="4">
                         <c:v>Dynamic</c:v>
@@ -1910,7 +1924,7 @@
                           <c15:sqref>Tabelle1!$G$6:$G$33</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(Tabelle1!$G$8,Tabelle1!$G$11,Tabelle1!$G$14,Tabelle1!$G$17,Tabelle1!$G$26,Tabelle1!$G$29,Tabelle1!$G$32)</c15:sqref>
+                          <c15:sqref>(Tabelle1!$G$8,Tabelle1!$G$11,Tabelle1!$G$14,Tabelle1!$G$20,Tabelle1!$G$26,Tabelle1!$G$29,Tabelle1!$G$32)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1947,7 +1961,7 @@
         </c:extLst>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-94638256"/>
+        <c:axId val="1516397440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1990,7 +2004,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-94643152"/>
+        <c:crossAx val="1516394176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1998,7 +2012,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-94643152"/>
+        <c:axId val="1516394176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2049,7 +2063,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-94638256"/>
+        <c:crossAx val="1516397440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2208,7 +2222,7 @@
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Tabelle1!$B$9,Tabelle1!$B$12,Tabelle1!$B$15,Tabelle1!$B$18,Tabelle1!$B$27,Tabelle1!$B$30,Tabelle1!$B$33)</c:f>
+              <c:f>(Tabelle1!$B$9,Tabelle1!$B$12,Tabelle1!$B$15,Tabelle1!$B$21,Tabelle1!$B$27,Tabelle1!$B$30,Tabelle1!$B$33)</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -2221,7 +2235,7 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>4.1</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>Dynamic</c:v>
@@ -2244,7 +2258,7 @@
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Tabelle1!$F$9,Tabelle1!$F$12,Tabelle1!$F$15,Tabelle1!$F$18,Tabelle1!$F$27,Tabelle1!$F$30,Tabelle1!$F$33)</c:f>
+              <c:f>(Tabelle1!$F$9,Tabelle1!$F$12,Tabelle1!$F$15,Tabelle1!$F$21,Tabelle1!$F$27,Tabelle1!$F$30,Tabelle1!$F$33)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -2283,8 +2297,8 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-94638800"/>
-        <c:axId val="-94645328"/>
+        <c:axId val="1516386016"/>
+        <c:axId val="1516396352"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredBarSeries>
@@ -2326,7 +2340,7 @@
                           <c15:sqref>Tabelle1!$B$6:$B$33</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(Tabelle1!$B$9,Tabelle1!$B$12,Tabelle1!$B$15,Tabelle1!$B$18,Tabelle1!$B$27,Tabelle1!$B$30,Tabelle1!$B$33)</c15:sqref>
+                          <c15:sqref>(Tabelle1!$B$9,Tabelle1!$B$12,Tabelle1!$B$15,Tabelle1!$B$21,Tabelle1!$B$27,Tabelle1!$B$30,Tabelle1!$B$33)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -2342,7 +2356,7 @@
                         <c:v>3</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>4</c:v>
+                        <c:v>4.1</c:v>
                       </c:pt>
                       <c:pt idx="4">
                         <c:v>Dynamic</c:v>
@@ -2364,7 +2378,7 @@
                           <c15:sqref>Tabelle1!$C$6:$C$33</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(Tabelle1!$C$9,Tabelle1!$C$12,Tabelle1!$C$15,Tabelle1!$C$18,Tabelle1!$C$27,Tabelle1!$C$30,Tabelle1!$C$33)</c15:sqref>
+                          <c15:sqref>(Tabelle1!$C$9,Tabelle1!$C$12,Tabelle1!$C$15,Tabelle1!$C$21,Tabelle1!$C$27,Tabelle1!$C$30,Tabelle1!$C$33)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -2381,13 +2395,16 @@
                         <c:v>3.4630000000000001</c:v>
                       </c:pt>
                       <c:pt idx="3" formatCode="0.00000">
-                        <c:v>2.4160599999999999</c:v>
+                        <c:v>4.8210899999999999</c:v>
                       </c:pt>
                       <c:pt idx="4" formatCode="0.00000">
                         <c:v>3.8240875000000001</c:v>
                       </c:pt>
                       <c:pt idx="5" formatCode="0.00000">
                         <c:v>5.6079650000000001</c:v>
+                      </c:pt>
+                      <c:pt idx="6" formatCode="0.00000">
+                        <c:v>0</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2400,7 +2417,7 @@
                 <c:order val="1"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Tabelle1!$D$5</c15:sqref>
@@ -2433,7 +2450,7 @@
                           <c15:sqref>Tabelle1!$B$6:$B$33</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(Tabelle1!$B$9,Tabelle1!$B$12,Tabelle1!$B$15,Tabelle1!$B$18,Tabelle1!$B$27,Tabelle1!$B$30,Tabelle1!$B$33)</c15:sqref>
+                          <c15:sqref>(Tabelle1!$B$9,Tabelle1!$B$12,Tabelle1!$B$15,Tabelle1!$B$21,Tabelle1!$B$27,Tabelle1!$B$30,Tabelle1!$B$33)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -2449,7 +2466,7 @@
                         <c:v>3</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>4</c:v>
+                        <c:v>4.1</c:v>
                       </c:pt>
                       <c:pt idx="4">
                         <c:v>Dynamic</c:v>
@@ -2471,7 +2488,7 @@
                           <c15:sqref>Tabelle1!$D$6:$D$33</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(Tabelle1!$D$9,Tabelle1!$D$12,Tabelle1!$D$15,Tabelle1!$D$18,Tabelle1!$D$27,Tabelle1!$D$30,Tabelle1!$D$33)</c15:sqref>
+                          <c15:sqref>(Tabelle1!$D$9,Tabelle1!$D$12,Tabelle1!$D$15,Tabelle1!$D$21,Tabelle1!$D$27,Tabelle1!$D$30,Tabelle1!$D$33)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -2488,13 +2505,16 @@
                         <c:v>2.6963900000000001</c:v>
                       </c:pt>
                       <c:pt idx="3" formatCode="0.00000">
-                        <c:v>2.8530249999999997</c:v>
+                        <c:v>2.0138775</c:v>
                       </c:pt>
                       <c:pt idx="4" formatCode="0.00000">
                         <c:v>2.2293775</c:v>
                       </c:pt>
                       <c:pt idx="5" formatCode="0.00000">
                         <c:v>3.4846724999999994</c:v>
+                      </c:pt>
+                      <c:pt idx="6" formatCode="0.00000">
+                        <c:v>0</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2507,7 +2527,7 @@
                 <c:order val="2"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Tabelle1!$E$5</c15:sqref>
@@ -2540,7 +2560,7 @@
                           <c15:sqref>Tabelle1!$B$6:$B$33</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(Tabelle1!$B$9,Tabelle1!$B$12,Tabelle1!$B$15,Tabelle1!$B$18,Tabelle1!$B$27,Tabelle1!$B$30,Tabelle1!$B$33)</c15:sqref>
+                          <c15:sqref>(Tabelle1!$B$9,Tabelle1!$B$12,Tabelle1!$B$15,Tabelle1!$B$21,Tabelle1!$B$27,Tabelle1!$B$30,Tabelle1!$B$33)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -2556,7 +2576,7 @@
                         <c:v>3</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>4</c:v>
+                        <c:v>4.1</c:v>
                       </c:pt>
                       <c:pt idx="4">
                         <c:v>Dynamic</c:v>
@@ -2578,7 +2598,7 @@
                           <c15:sqref>Tabelle1!$E$6:$E$33</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(Tabelle1!$E$9,Tabelle1!$E$12,Tabelle1!$E$15,Tabelle1!$E$18,Tabelle1!$E$27,Tabelle1!$E$30,Tabelle1!$E$33)</c15:sqref>
+                          <c15:sqref>(Tabelle1!$E$9,Tabelle1!$E$12,Tabelle1!$E$15,Tabelle1!$E$21,Tabelle1!$E$27,Tabelle1!$E$30,Tabelle1!$E$33)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -2595,13 +2615,16 @@
                         <c:v>0.76924999999999999</c:v>
                       </c:pt>
                       <c:pt idx="3" formatCode="0.00000">
-                        <c:v>1.7616400000000001</c:v>
+                        <c:v>2.47004</c:v>
                       </c:pt>
                       <c:pt idx="4" formatCode="0.00000">
                         <c:v>0.77546300000000001</c:v>
                       </c:pt>
                       <c:pt idx="5" formatCode="0.00000">
                         <c:v>2.7390800000000004</c:v>
+                      </c:pt>
+                      <c:pt idx="6" formatCode="0.00000">
+                        <c:v>0</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -2614,7 +2637,7 @@
                 <c:order val="4"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Tabelle1!$G$5</c15:sqref>
@@ -2647,7 +2670,7 @@
                           <c15:sqref>Tabelle1!$B$6:$B$33</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(Tabelle1!$B$9,Tabelle1!$B$12,Tabelle1!$B$15,Tabelle1!$B$18,Tabelle1!$B$27,Tabelle1!$B$30,Tabelle1!$B$33)</c15:sqref>
+                          <c15:sqref>(Tabelle1!$B$9,Tabelle1!$B$12,Tabelle1!$B$15,Tabelle1!$B$21,Tabelle1!$B$27,Tabelle1!$B$30,Tabelle1!$B$33)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -2663,7 +2686,7 @@
                         <c:v>3</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>4</c:v>
+                        <c:v>4.1</c:v>
                       </c:pt>
                       <c:pt idx="4">
                         <c:v>Dynamic</c:v>
@@ -2685,7 +2708,7 @@
                           <c15:sqref>Tabelle1!$G$6:$G$33</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(Tabelle1!$G$9,Tabelle1!$G$12,Tabelle1!$G$15,Tabelle1!$G$18,Tabelle1!$G$27,Tabelle1!$G$30,Tabelle1!$G$33)</c15:sqref>
+                          <c15:sqref>(Tabelle1!$G$9,Tabelle1!$G$12,Tabelle1!$G$15,Tabelle1!$G$21,Tabelle1!$G$27,Tabelle1!$G$30,Tabelle1!$G$33)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -2722,7 +2745,7 @@
         </c:extLst>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-94638800"/>
+        <c:axId val="1516386016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2765,7 +2788,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-94645328"/>
+        <c:crossAx val="1516396352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2773,7 +2796,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-94645328"/>
+        <c:axId val="1516396352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2824,7 +2847,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-94638800"/>
+        <c:crossAx val="1516386016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3046,11 +3069,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-160220016"/>
-        <c:axId val="-160217840"/>
+        <c:axId val="1465944400"/>
+        <c:axId val="1514719792"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-160220016"/>
+        <c:axId val="1465944400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3068,7 +3091,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="-160217840"/>
+        <c:crossAx val="1514719792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3076,7 +3099,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-160217840"/>
+        <c:axId val="1514719792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3101,7 +3124,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="-160220016"/>
+        <c:crossAx val="1465944400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.1"/>
@@ -3317,11 +3340,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-160211856"/>
-        <c:axId val="-288279632"/>
+        <c:axId val="1514714896"/>
+        <c:axId val="1514711632"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-160211856"/>
+        <c:axId val="1514714896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3339,7 +3362,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="-288279632"/>
+        <c:crossAx val="1514711632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3347,7 +3370,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-288279632"/>
+        <c:axId val="1514711632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3372,7 +3395,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="-160211856"/>
+        <c:crossAx val="1514714896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -3943,8 +3966,14 @@
                 <c:pt idx="2" formatCode="0.00000">
                   <c:v>4.7090099999999993</c:v>
                 </c:pt>
-                <c:pt idx="3" formatCode="0.00000">
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0.00000">
                   <c:v>2.9464066666666664</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="0.00000">
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="0.00000">
                   <c:v>3.1262899999999996</c:v>
@@ -4037,8 +4066,14 @@
                 <c:pt idx="2" formatCode="0.00000">
                   <c:v>24.8612</c:v>
                 </c:pt>
-                <c:pt idx="3" formatCode="0.00000">
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0.00000">
                   <c:v>10.622866666666667</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="0.00000">
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="0.00000">
                   <c:v>10.492599999999999</c:v>
@@ -4060,11 +4095,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-96053232"/>
-        <c:axId val="-96051600"/>
+        <c:axId val="1514707824"/>
+        <c:axId val="1514715440"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-96053232"/>
+        <c:axId val="1514707824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4082,7 +4117,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="-96051600"/>
+        <c:crossAx val="1514715440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4090,7 +4125,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-96051600"/>
+        <c:axId val="1514715440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4115,7 +4150,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="-96053232"/>
+        <c:crossAx val="1514707824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -4348,11 +4383,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-96048880"/>
-        <c:axId val="-96047792"/>
+        <c:axId val="1514712720"/>
+        <c:axId val="1514717072"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-96048880"/>
+        <c:axId val="1514712720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4370,7 +4405,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="-96047792"/>
+        <c:crossAx val="1514717072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4378,7 +4413,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-96047792"/>
+        <c:axId val="1514717072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4403,7 +4438,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="-96048880"/>
+        <c:crossAx val="1514712720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.25"/>
@@ -4611,11 +4646,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-96061392"/>
-        <c:axId val="-96047248"/>
+        <c:axId val="1514708368"/>
+        <c:axId val="1514718160"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-96061392"/>
+        <c:axId val="1514708368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4633,7 +4668,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="-96047248"/>
+        <c:crossAx val="1514718160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4641,7 +4676,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-96047248"/>
+        <c:axId val="1514718160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4666,7 +4701,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="-96061392"/>
+        <c:crossAx val="1514708368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.5"/>
@@ -4882,11 +4917,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-96051056"/>
-        <c:axId val="-96054320"/>
+        <c:axId val="1514722512"/>
+        <c:axId val="1514708912"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-96051056"/>
+        <c:axId val="1514722512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4904,7 +4939,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="-96054320"/>
+        <c:crossAx val="1514708912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4912,7 +4947,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-96054320"/>
+        <c:axId val="1514708912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4937,7 +4972,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="-96051056"/>
+        <c:crossAx val="1514722512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.25"/>
@@ -5425,8 +5460,14 @@
                 <c:pt idx="2" formatCode="0.00000">
                   <c:v>0.3609093333333333</c:v>
                 </c:pt>
-                <c:pt idx="3" formatCode="0.00000">
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0.00000">
                   <c:v>0.59135633333333326</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="0.00000">
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="0.00000">
                   <c:v>0.56800899999999999</c:v>
@@ -5519,8 +5560,14 @@
                 <c:pt idx="2" formatCode="0.00000">
                   <c:v>6.5944533333333333E-2</c:v>
                 </c:pt>
-                <c:pt idx="3" formatCode="0.00000">
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0.00000">
                   <c:v>0.156558</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="0.00000">
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="0.00000">
                   <c:v>0.15804766666666667</c:v>
@@ -5542,11 +5589,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-96058672"/>
-        <c:axId val="-96062480"/>
+        <c:axId val="1514709456"/>
+        <c:axId val="1514710000"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-96058672"/>
+        <c:axId val="1514709456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5564,7 +5611,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="-96062480"/>
+        <c:crossAx val="1514710000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5572,7 +5619,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-96062480"/>
+        <c:axId val="1514710000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5597,7 +5644,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="-96058672"/>
+        <c:crossAx val="1514709456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5756,7 +5803,7 @@
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Tabelle1!$B$8,Tabelle1!$B$11,Tabelle1!$B$14,Tabelle1!$B$17,Tabelle1!$B$26,Tabelle1!$B$29,Tabelle1!$B$32)</c:f>
+              <c:f>(Tabelle1!$B$8,Tabelle1!$B$11,Tabelle1!$B$14,Tabelle1!$B$20,Tabelle1!$B$26,Tabelle1!$B$29,Tabelle1!$B$32)</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -5769,7 +5816,7 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>4.1</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>Dynamic</c:v>
@@ -5792,7 +5839,7 @@
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>(Tabelle1!$G$8,Tabelle1!$G$11,Tabelle1!$G$14,Tabelle1!$G$17,Tabelle1!$G$26,Tabelle1!$G$29,Tabelle1!$G$32)</c:f>
+              <c:f>(Tabelle1!$G$8,Tabelle1!$G$11,Tabelle1!$G$14,Tabelle1!$G$20,Tabelle1!$G$26,Tabelle1!$G$29,Tabelle1!$G$32)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -5831,8 +5878,8 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-96060848"/>
-        <c:axId val="-96060304"/>
+        <c:axId val="1514712176"/>
+        <c:axId val="1514716528"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredBarSeries>
@@ -5874,7 +5921,7 @@
                           <c15:sqref>Tabelle1!$B$6:$B$33</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(Tabelle1!$B$8,Tabelle1!$B$11,Tabelle1!$B$14,Tabelle1!$B$17,Tabelle1!$B$26,Tabelle1!$B$29,Tabelle1!$B$32)</c15:sqref>
+                          <c15:sqref>(Tabelle1!$B$8,Tabelle1!$B$11,Tabelle1!$B$14,Tabelle1!$B$20,Tabelle1!$B$26,Tabelle1!$B$29,Tabelle1!$B$32)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -5890,7 +5937,7 @@
                         <c:v>3</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>4</c:v>
+                        <c:v>4.1</c:v>
                       </c:pt>
                       <c:pt idx="4">
                         <c:v>Dynamic</c:v>
@@ -5912,7 +5959,7 @@
                           <c15:sqref>Tabelle1!$C$6:$C$33</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(Tabelle1!$C$8,Tabelle1!$C$11,Tabelle1!$C$14,Tabelle1!$C$17,Tabelle1!$C$26,Tabelle1!$C$29,Tabelle1!$C$32)</c15:sqref>
+                          <c15:sqref>(Tabelle1!$C$8,Tabelle1!$C$11,Tabelle1!$C$14,Tabelle1!$C$20,Tabelle1!$C$26,Tabelle1!$C$29,Tabelle1!$C$32)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -5929,13 +5976,16 @@
                         <c:v>0.69523500000000005</c:v>
                       </c:pt>
                       <c:pt idx="3" formatCode="0.00000">
-                        <c:v>1.0202374999999999</c:v>
+                        <c:v>0.5261922</c:v>
                       </c:pt>
                       <c:pt idx="4" formatCode="0.00000">
                         <c:v>0.64015949999999999</c:v>
                       </c:pt>
                       <c:pt idx="5" formatCode="0.00000">
                         <c:v>0.41012674999999998</c:v>
+                      </c:pt>
+                      <c:pt idx="6" formatCode="0.00000">
+                        <c:v>0</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -5948,7 +5998,7 @@
                 <c:order val="1"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Tabelle1!$D$5</c15:sqref>
@@ -5981,7 +6031,7 @@
                           <c15:sqref>Tabelle1!$B$6:$B$33</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(Tabelle1!$B$8,Tabelle1!$B$11,Tabelle1!$B$14,Tabelle1!$B$17,Tabelle1!$B$26,Tabelle1!$B$29,Tabelle1!$B$32)</c15:sqref>
+                          <c15:sqref>(Tabelle1!$B$8,Tabelle1!$B$11,Tabelle1!$B$14,Tabelle1!$B$20,Tabelle1!$B$26,Tabelle1!$B$29,Tabelle1!$B$32)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -5997,7 +6047,7 @@
                         <c:v>3</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>4</c:v>
+                        <c:v>4.1</c:v>
                       </c:pt>
                       <c:pt idx="4">
                         <c:v>Dynamic</c:v>
@@ -6019,7 +6069,7 @@
                           <c15:sqref>Tabelle1!$D$6:$D$33</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(Tabelle1!$D$8,Tabelle1!$D$11,Tabelle1!$D$14,Tabelle1!$D$17,Tabelle1!$D$26,Tabelle1!$D$29,Tabelle1!$D$32)</c15:sqref>
+                          <c15:sqref>(Tabelle1!$D$8,Tabelle1!$D$11,Tabelle1!$D$14,Tabelle1!$D$20,Tabelle1!$D$26,Tabelle1!$D$29,Tabelle1!$D$32)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -6036,13 +6086,16 @@
                         <c:v>0.69224300000000005</c:v>
                       </c:pt>
                       <c:pt idx="3" formatCode="0.00000">
-                        <c:v>0.65996350000000004</c:v>
+                        <c:v>0.89916050000000003</c:v>
                       </c:pt>
                       <c:pt idx="4" formatCode="0.00000">
                         <c:v>0.81985074999999996</c:v>
                       </c:pt>
                       <c:pt idx="5" formatCode="0.00000">
                         <c:v>0.55638799999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="6" formatCode="0.00000">
+                        <c:v>0</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -6055,7 +6108,7 @@
                 <c:order val="2"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Tabelle1!$E$5</c15:sqref>
@@ -6088,7 +6141,7 @@
                           <c15:sqref>Tabelle1!$B$6:$B$33</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(Tabelle1!$B$8,Tabelle1!$B$11,Tabelle1!$B$14,Tabelle1!$B$17,Tabelle1!$B$26,Tabelle1!$B$29,Tabelle1!$B$32)</c15:sqref>
+                          <c15:sqref>(Tabelle1!$B$8,Tabelle1!$B$11,Tabelle1!$B$14,Tabelle1!$B$20,Tabelle1!$B$26,Tabelle1!$B$29,Tabelle1!$B$32)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -6104,7 +6157,7 @@
                         <c:v>3</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>4</c:v>
+                        <c:v>4.1</c:v>
                       </c:pt>
                       <c:pt idx="4">
                         <c:v>Dynamic</c:v>
@@ -6126,7 +6179,7 @@
                           <c15:sqref>Tabelle1!$E$6:$E$33</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(Tabelle1!$E$8,Tabelle1!$E$11,Tabelle1!$E$14,Tabelle1!$E$17,Tabelle1!$E$26,Tabelle1!$E$29,Tabelle1!$E$32)</c15:sqref>
+                          <c15:sqref>(Tabelle1!$E$8,Tabelle1!$E$11,Tabelle1!$E$14,Tabelle1!$E$20,Tabelle1!$E$26,Tabelle1!$E$29,Tabelle1!$E$32)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -6143,13 +6196,16 @@
                         <c:v>2.15306</c:v>
                       </c:pt>
                       <c:pt idx="3" formatCode="0.00000">
-                        <c:v>1.1096766666666669</c:v>
+                        <c:v>0.84413766666666668</c:v>
                       </c:pt>
                       <c:pt idx="4" formatCode="0.00000">
                         <c:v>2.3757225000000002</c:v>
                       </c:pt>
                       <c:pt idx="5" formatCode="0.00000">
                         <c:v>0.7935812499999999</c:v>
+                      </c:pt>
+                      <c:pt idx="6" formatCode="0.00000">
+                        <c:v>0</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -6162,7 +6218,7 @@
                 <c:order val="3"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Tabelle1!$F$5</c15:sqref>
@@ -6195,7 +6251,7 @@
                           <c15:sqref>Tabelle1!$B$6:$B$33</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(Tabelle1!$B$8,Tabelle1!$B$11,Tabelle1!$B$14,Tabelle1!$B$17,Tabelle1!$B$26,Tabelle1!$B$29,Tabelle1!$B$32)</c15:sqref>
+                          <c15:sqref>(Tabelle1!$B$8,Tabelle1!$B$11,Tabelle1!$B$14,Tabelle1!$B$20,Tabelle1!$B$26,Tabelle1!$B$29,Tabelle1!$B$32)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -6211,7 +6267,7 @@
                         <c:v>3</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>4</c:v>
+                        <c:v>4.1</c:v>
                       </c:pt>
                       <c:pt idx="4">
                         <c:v>Dynamic</c:v>
@@ -6233,7 +6289,7 @@
                           <c15:sqref>Tabelle1!$F$6:$F$33</c15:sqref>
                         </c15:fullRef>
                         <c15:formulaRef>
-                          <c15:sqref>(Tabelle1!$F$8,Tabelle1!$F$11,Tabelle1!$F$14,Tabelle1!$F$17,Tabelle1!$F$26,Tabelle1!$F$29,Tabelle1!$F$32)</c15:sqref>
+                          <c15:sqref>(Tabelle1!$F$8,Tabelle1!$F$11,Tabelle1!$F$14,Tabelle1!$F$20,Tabelle1!$F$26,Tabelle1!$F$29,Tabelle1!$F$32)</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -6270,7 +6326,7 @@
         </c:extLst>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-96060848"/>
+        <c:axId val="1514712176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6313,7 +6369,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-96060304"/>
+        <c:crossAx val="1514716528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6321,7 +6377,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-96060304"/>
+        <c:axId val="1514716528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6372,7 +6428,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-96060848"/>
+        <c:crossAx val="1514712176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="5"/>
@@ -9224,8 +9280,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:I35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R83" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Z125" sqref="Z125"/>
+    <sheetView tabSelected="1" topLeftCell="M87" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AM129" sqref="AM129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9320,24 +9376,24 @@
       <c r="B8" s="3">
         <v>1</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="6">
         <v>0.53157466669999998</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="6">
         <v>8.1672499999999992</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="6">
         <v>19.013000000000002</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="6">
         <f>(5.04545+ 5.01575+5.02542)/3</f>
         <v>5.0288733333333333</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="6">
         <f>(59.0787+58.6633+58.6611)/3</f>
         <v>58.801033333333329</v>
       </c>
-      <c r="H8" s="5" t="s">
+      <c r="H8" s="4" t="s">
         <v>10</v>
       </c>
     </row>
@@ -9345,41 +9401,41 @@
       <c r="B9" s="3">
         <v>1</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="3">
         <v>4.9249099999999997</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="6">
         <v>0.21723400000000001</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="6">
         <v>8.5662699999999994E-2</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="6">
         <f>(0.334904+0.337114+0.336987)/3</f>
         <v>0.336335</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="6">
         <f>(0.0276139+0.0278119+0.027812)/3</f>
         <v>2.7745933333333334E-2</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="H9" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B10" s="3"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="5"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="4"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
         <v>2</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="6">
         <f>(0.481526+0.482208+0.4843+0.483932)/4</f>
         <v>0.48299150000000002</v>
       </c>
@@ -9387,18 +9443,18 @@
         <f>(0.57981+0.57683+0.581912+0.578102)/4</f>
         <v>0.57916349999999994</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="6">
         <v>0.77977624999999995</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11" s="6">
         <f>(1.91642+1.87226+1.95972)/3</f>
         <v>1.9161333333333335</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G11" s="6">
         <f>(5.92878+5.70786+5.65863)/3</f>
         <v>5.7650899999999998</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="H11" s="4" t="s">
         <v>10</v>
       </c>
     </row>
@@ -9406,7 +9462,7 @@
       <c r="B12" s="3">
         <v>2</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="6">
         <f>(5.22963+5.24131+5.19444+5.21264)/4</f>
         <v>5.2195049999999998</v>
       </c>
@@ -9414,52 +9470,52 @@
         <f>(3.34028+3.34108+3.33607+3.33492)/4</f>
         <v>3.3380874999999999</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="6">
         <v>2.7210800000000002</v>
       </c>
-      <c r="F12" s="4">
+      <c r="F12" s="6">
         <f>(0.94405+0.970787+0.918559)/3</f>
         <v>0.94446533333333338</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G12" s="6">
         <f>(0.295786+0.295444+0.297827)/3</f>
         <v>0.29635233333333333</v>
       </c>
-      <c r="H12" s="5" t="s">
+      <c r="H12" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B13" s="3"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="5"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="4"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B14" s="3">
         <v>3</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14" s="6">
         <v>0.69523500000000005</v>
       </c>
-      <c r="D14" s="4">
+      <c r="D14" s="6">
         <v>0.69224300000000005</v>
       </c>
-      <c r="E14" s="4">
+      <c r="E14" s="6">
         <v>2.15306</v>
       </c>
-      <c r="F14" s="4">
+      <c r="F14" s="6">
         <f>(4.80821+4.72045+4.59837)/3</f>
         <v>4.7090099999999993</v>
       </c>
-      <c r="G14" s="4">
+      <c r="G14" s="6">
         <f>(24.8308+24.8794+24.8734)/3</f>
         <v>24.8612</v>
       </c>
-      <c r="H14" s="5" t="s">
+      <c r="H14" s="4" t="s">
         <v>10</v>
       </c>
     </row>
@@ -9467,41 +9523,41 @@
       <c r="B15" s="3">
         <v>3</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15" s="6">
         <v>3.4630000000000001</v>
       </c>
-      <c r="D15" s="4">
+      <c r="D15" s="6">
         <v>2.6963900000000001</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E15" s="6">
         <v>0.76924999999999999</v>
       </c>
-      <c r="F15" s="4">
+      <c r="F15" s="6">
         <f>(0.352992+0.359944+0.369792)/3</f>
         <v>0.3609093333333333</v>
       </c>
-      <c r="G15" s="4">
+      <c r="G15" s="6">
         <f>(0.0660048+0.0659163+0.0659125)/3</f>
         <v>6.5944533333333333E-2</v>
       </c>
-      <c r="H15" s="5" t="s">
+      <c r="H15" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B16" s="3"/>
-      <c r="C16" s="4"/>
+      <c r="C16" s="6"/>
       <c r="D16" s="6"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="5"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="4"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B17" s="3">
         <v>4</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C17" s="6">
         <f>(1.01107+1.0242+1.0322+1.01348)/4</f>
         <v>1.0202374999999999</v>
       </c>
@@ -9509,19 +9565,17 @@
         <f>(0.661035+0.660433+0.660824+0.657562)/4</f>
         <v>0.65996350000000004</v>
       </c>
-      <c r="E17" s="4">
+      <c r="E17" s="6">
         <f>(1.10844+1.1032+1.11739)/3</f>
         <v>1.1096766666666669</v>
       </c>
-      <c r="F17" s="4">
-        <f>(2.92011+3.04471+2.8744)/3</f>
-        <v>2.9464066666666664</v>
-      </c>
-      <c r="G17" s="4">
-        <f>(10.66+10.5578+10.6508)/3</f>
-        <v>10.622866666666667</v>
-      </c>
-      <c r="H17" s="5" t="s">
+      <c r="F17" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H17" s="4" t="s">
         <v>10</v>
       </c>
       <c r="I17" t="s">
@@ -9532,55 +9586,59 @@
       <c r="B18" s="3">
         <v>4</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C18" s="6">
         <v>2.4160599999999999</v>
       </c>
       <c r="D18" s="6">
         <f>(2.85531+2.85449+2.84999+2.85231)/4</f>
         <v>2.8530249999999997</v>
       </c>
-      <c r="E18" s="4">
+      <c r="E18" s="6">
         <v>1.7616400000000001</v>
       </c>
-      <c r="F18" s="4">
-        <f>(0.595737+0.570898+0.607434)/3</f>
-        <v>0.59135633333333326</v>
-      </c>
-      <c r="G18" s="4">
-        <f>(0.155611+0.157066+0.156997)/3</f>
-        <v>0.156558</v>
-      </c>
-      <c r="H18" s="5" t="s">
+      <c r="F18" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H18" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B19" s="3"/>
-      <c r="C19" s="4"/>
+      <c r="C19" s="6"/>
       <c r="D19" s="6"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="5"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="4"/>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C20" s="4">
+      <c r="C20" s="6">
         <v>0.5261922</v>
       </c>
       <c r="D20" s="6">
         <f>(0.899913+0.899776+0.895833+0.90112)/4</f>
         <v>0.89916050000000003</v>
       </c>
-      <c r="E20" s="4">
+      <c r="E20" s="6">
         <f>(0.850354+0.842024+0.840035)/3</f>
         <v>0.84413766666666668</v>
       </c>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="5" t="s">
+      <c r="F20" s="6">
+        <f>(2.92011+3.04471+2.8744)/3</f>
+        <v>2.9464066666666664</v>
+      </c>
+      <c r="G20" s="6">
+        <f>(10.66+10.5578+10.6508)/3</f>
+        <v>10.622866666666667</v>
+      </c>
+      <c r="H20" s="4" t="s">
         <v>10</v>
       </c>
       <c r="I20" t="s">
@@ -9588,51 +9646,61 @@
       </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B21" s="7" t="s">
+      <c r="B21" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C21" s="4">
+      <c r="C21" s="6">
         <v>4.8210899999999999</v>
       </c>
       <c r="D21" s="6">
         <f>(2.01356+2.01146+2.01594+2.01455)/4</f>
         <v>2.0138775</v>
       </c>
-      <c r="E21" s="4">
+      <c r="E21" s="6">
         <v>2.47004</v>
       </c>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
+      <c r="F21" s="6">
+        <f>(0.595737+0.570898+0.607434)/3</f>
+        <v>0.59135633333333326</v>
+      </c>
+      <c r="G21" s="6">
+        <f>(0.155611+0.157066+0.156997)/3</f>
+        <v>0.156558</v>
+      </c>
       <c r="H21" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B22" s="3"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B23" s="7" t="s">
+      <c r="B23" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C23" s="4">
+      <c r="C23" s="6">
         <f>(1.4547+1.47025+1.49688)/4</f>
         <v>1.1054575</v>
       </c>
-      <c r="D23" s="8" t="s">
+      <c r="D23" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E23" s="4">
+      <c r="E23" s="6">
         <f>(2.33107+2.35205+2.35205+2.48147+2.30158)/4</f>
         <v>2.954555</v>
       </c>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="5" t="s">
+      <c r="F23" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H23" s="4" t="s">
         <v>10</v>
       </c>
       <c r="I23" t="s">
@@ -9640,53 +9708,57 @@
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B24" s="7" t="s">
+      <c r="B24" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="4">
+      <c r="C24" s="6">
         <v>1.4354499999999999</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="D24" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E24" s="4">
+      <c r="E24" s="6">
         <v>0.75661400000000001</v>
       </c>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="5" t="s">
+      <c r="F24" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H24" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B25" s="3"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B26" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C26" s="8">
+      <c r="C26" s="6">
         <f>(0.60382+0.61476+0.604918+0.73714)/4</f>
         <v>0.64015949999999999</v>
       </c>
-      <c r="D26" s="8">
+      <c r="D26" s="6">
         <f>(0.818113+0.823809+0.819304+0.818177)/4</f>
         <v>0.81985074999999996</v>
       </c>
-      <c r="E26" s="8">
+      <c r="E26" s="6">
         <f>(2.56391+2.31429+2.30321+2.32148)/4</f>
         <v>2.3757225000000002</v>
       </c>
-      <c r="F26" s="8">
+      <c r="F26" s="6">
         <f>(2.97241+3.60945+2.79701)/3</f>
         <v>3.1262899999999996</v>
       </c>
-      <c r="G26" s="8">
+      <c r="G26" s="6">
         <f>(10.5706+10.4424+10.4648)/3</f>
         <v>10.492599999999999</v>
       </c>
@@ -9698,23 +9770,23 @@
       <c r="B27" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C27" s="8">
+      <c r="C27" s="6">
         <f>(3.77988+3.71921+3.76059+4.03667 )/4</f>
         <v>3.8240875000000001</v>
       </c>
-      <c r="D27" s="8">
+      <c r="D27" s="6">
         <f>(2.22981+2.22904+2.22949+2.22917)/4</f>
         <v>2.2293775</v>
       </c>
-      <c r="E27" s="8">
+      <c r="E27" s="6">
         <f>(0.722009+0.794159+0.795563 +0.790121 )/4</f>
         <v>0.77546300000000001</v>
       </c>
-      <c r="F27" s="8">
+      <c r="F27" s="6">
         <f>(0.591431+0.480298+0.632298)/3</f>
         <v>0.56800899999999999</v>
       </c>
-      <c r="G27" s="8">
+      <c r="G27" s="6">
         <f>(0.156844+0.158761+0.158538)/3</f>
         <v>0.15804766666666667</v>
       </c>
@@ -9724,34 +9796,34 @@
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B28" s="3"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
       <c r="H28" s="3"/>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B29" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C29" s="8">
+      <c r="C29" s="6">
         <f>(0.38893+0.428742+0.411657+0.411178)/4</f>
         <v>0.41012674999999998</v>
       </c>
-      <c r="D29" s="8">
+      <c r="D29" s="6">
         <f>(0.556837+0.555766+0.559186+0.553763)/4</f>
         <v>0.55638799999999999</v>
       </c>
-      <c r="E29" s="8">
+      <c r="E29" s="6">
         <f>(0.770456+0.80318+0.798453+0.802236)/4</f>
         <v>0.7935812499999999</v>
       </c>
-      <c r="F29" s="8">
+      <c r="F29" s="6">
         <f>(1.82445+1.82329+1.81177)/3</f>
         <v>1.8198366666666665</v>
       </c>
-      <c r="G29" s="8">
+      <c r="G29" s="6">
         <f>(5.78958+5.79993+5.76721)/3</f>
         <v>5.7855733333333346</v>
       </c>
@@ -9760,26 +9832,26 @@
       </c>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B30" s="9" t="s">
+      <c r="B30" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C30" s="8">
+      <c r="C30" s="6">
         <f>(5.94859+5.16703+5.60233+5.71391)/4</f>
         <v>5.6079650000000001</v>
       </c>
-      <c r="D30" s="8">
+      <c r="D30" s="6">
         <f>(3.48563+3.48459+3.48599+3.48248)/4</f>
         <v>3.4846724999999994</v>
       </c>
-      <c r="E30" s="10">
+      <c r="E30" s="8">
         <f>(2.78492+2.71566+2.71721+2.73853)/4</f>
         <v>2.7390800000000004</v>
       </c>
-      <c r="F30" s="10">
+      <c r="F30" s="8">
         <f>(0.957571+0.954979+0.962367)/3</f>
         <v>0.95830566666666661</v>
       </c>
-      <c r="G30" s="10">
+      <c r="G30" s="8">
         <f>(0.287421+0.286989+0.288813)/3</f>
         <v>0.28774099999999997</v>
       </c>
@@ -9788,24 +9860,30 @@
       </c>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="8"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="8"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B32" s="9" t="s">
+      <c r="B32" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C32" s="8"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="8"/>
-      <c r="F32" s="8">
+      <c r="C32" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F32" s="6">
         <f>(14.0429+14.0905+14.0542)/3</f>
         <v>14.062533333333334</v>
       </c>
-      <c r="G32" s="8">
+      <c r="G32" s="6">
         <f>(50.2407+50.2457+50.2273)/3</f>
         <v>50.237900000000003</v>
       </c>
@@ -9817,17 +9895,23 @@
       </c>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B33" s="9" t="s">
+      <c r="B33" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8"/>
-      <c r="F33" s="8">
+      <c r="C33" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F33" s="6">
         <f>(((1.15767+1.15376+1.15673)/3)/1000)*100</f>
         <v>0.11560533333333331</v>
       </c>
-      <c r="G33" s="8">
+      <c r="G33" s="6">
         <f>((323583+323550+323669)/3)/10^9*100</f>
         <v>3.2360066666666673E-2</v>
       </c>

</xml_diff>

<commit_message>
Diagramm all 5point kernels added
</commit_message>
<xml_diff>
--- a/Output/Kernel vergleich.xlsx
+++ b/Output/Kernel vergleich.xlsx
@@ -484,11 +484,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1725961424"/>
-        <c:axId val="1725963600"/>
+        <c:axId val="-1740121952"/>
+        <c:axId val="-1740103456"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1725961424"/>
+        <c:axId val="-1740121952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -506,7 +506,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="1725963600"/>
+        <c:crossAx val="-1740103456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -514,7 +514,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1725963600"/>
+        <c:axId val="-1740103456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="20"/>
@@ -543,7 +543,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="1725961424"/>
+        <c:crossAx val="-1740121952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -763,8 +763,8 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1725981008"/>
-        <c:axId val="1725970672"/>
+        <c:axId val="-87666048"/>
+        <c:axId val="-1734637280"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredBarSeries>
@@ -1211,7 +1211,7 @@
         </c:extLst>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1725981008"/>
+        <c:axId val="-87666048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1254,7 +1254,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1725970672"/>
+        <c:crossAx val="-1734637280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1262,7 +1262,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1725970672"/>
+        <c:axId val="-1734637280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1313,7 +1313,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1725981008"/>
+        <c:crossAx val="-87666048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1551,8 +1551,8 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1725976656"/>
-        <c:axId val="1725982096"/>
+        <c:axId val="-1734637824"/>
+        <c:axId val="-1734634016"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredBarSeries>
@@ -1999,7 +1999,7 @@
         </c:extLst>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1725976656"/>
+        <c:axId val="-1734637824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2042,7 +2042,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1725982096"/>
+        <c:crossAx val="-1734634016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2050,7 +2050,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1725982096"/>
+        <c:axId val="-1734634016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2101,7 +2101,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1725976656"/>
+        <c:crossAx val="-1734637824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2335,8 +2335,8 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1725971216"/>
-        <c:axId val="1725972304"/>
+        <c:axId val="-1734629664"/>
+        <c:axId val="-1734628576"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredBarSeries>
@@ -2783,7 +2783,7 @@
         </c:extLst>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1725971216"/>
+        <c:axId val="-1734629664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2826,7 +2826,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1725972304"/>
+        <c:crossAx val="-1734628576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2834,7 +2834,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1725972304"/>
+        <c:axId val="-1734628576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2885,7 +2885,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1725971216"/>
+        <c:crossAx val="-1734629664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3738,11 +3738,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="-24"/>
-        <c:axId val="1725972848"/>
-        <c:axId val="1725973936"/>
+        <c:axId val="-1734632928"/>
+        <c:axId val="-1734631296"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1725972848"/>
+        <c:axId val="-1734632928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3784,7 +3784,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1725973936"/>
+        <c:crossAx val="-1734631296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3792,7 +3792,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1725973936"/>
+        <c:axId val="-1734631296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3896,7 +3896,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1725972848"/>
+        <c:crossAx val="-1734632928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4307,9 +4307,7 @@
                     <c:showPercent val="0"/>
                     <c:showBubbleSize val="0"/>
                     <c:extLst>
-                      <c:ext uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                        <c15:layout/>
-                      </c:ext>
+                      <c:ext uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                     </c:extLst>
                   </c15:dLbl>
                 </c15:categoryFilterException>
@@ -4625,9 +4623,7 @@
                     <c:showPercent val="0"/>
                     <c:showBubbleSize val="0"/>
                     <c:extLst>
-                      <c:ext uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                        <c15:layout/>
-                      </c:ext>
+                      <c:ext uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                     </c:extLst>
                   </c15:dLbl>
                 </c15:categoryFilterException>
@@ -4800,11 +4796,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="-24"/>
-        <c:axId val="1639817952"/>
-        <c:axId val="1639827744"/>
+        <c:axId val="-1734620416"/>
+        <c:axId val="-1734628032"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1639817952"/>
+        <c:axId val="-1734620416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4846,7 +4842,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1639827744"/>
+        <c:crossAx val="-1734628032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4854,7 +4850,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1639827744"/>
+        <c:axId val="-1734628032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4958,7 +4954,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1639817952"/>
+        <c:crossAx val="-1734620416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5248,9 +5244,7 @@
               <c:idx val="3"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -5543,9 +5537,7 @@
               <c:idx val="3"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -5718,9 +5710,7 @@
               <c:idx val="3"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -5846,11 +5836,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="-24"/>
-        <c:axId val="1160787136"/>
-        <c:axId val="1160787680"/>
+        <c:axId val="-1734627488"/>
+        <c:axId val="-1734631840"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1160787136"/>
+        <c:axId val="-1734627488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5892,7 +5882,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1160787680"/>
+        <c:crossAx val="-1734631840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5900,7 +5890,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1160787680"/>
+        <c:axId val="-1734631840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6004,7 +5994,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1160787136"/>
+        <c:crossAx val="-1734627488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6415,9 +6405,7 @@
                     <c:showPercent val="0"/>
                     <c:showBubbleSize val="0"/>
                     <c:extLst>
-                      <c:ext uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                        <c15:layout/>
-                      </c:ext>
+                      <c:ext uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                     </c:extLst>
                   </c15:dLbl>
                 </c15:categoryFilterException>
@@ -6733,9 +6721,7 @@
                     <c:showPercent val="0"/>
                     <c:showBubbleSize val="0"/>
                     <c:extLst>
-                      <c:ext uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                        <c15:layout/>
-                      </c:ext>
+                      <c:ext uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                     </c:extLst>
                   </c15:dLbl>
                 </c15:categoryFilterException>
@@ -6908,11 +6894,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="-24"/>
-        <c:axId val="947161216"/>
-        <c:axId val="947162304"/>
+        <c:axId val="-1734625312"/>
+        <c:axId val="-1734636736"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="947161216"/>
+        <c:axId val="-1734625312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6954,7 +6940,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="947162304"/>
+        <c:crossAx val="-1734636736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6962,7 +6948,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="947162304"/>
+        <c:axId val="-1734636736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7066,7 +7052,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="947161216"/>
+        <c:crossAx val="-1734625312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7489,9 +7475,7 @@
                     <c:showPercent val="0"/>
                     <c:showBubbleSize val="0"/>
                     <c:extLst>
-                      <c:ext uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                        <c15:layout/>
-                      </c:ext>
+                      <c:ext uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                     </c:extLst>
                   </c15:dLbl>
                 </c15:categoryFilterException>
@@ -7819,9 +7803,7 @@
                     <c:showPercent val="0"/>
                     <c:showBubbleSize val="0"/>
                     <c:extLst>
-                      <c:ext uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                        <c15:layout/>
-                      </c:ext>
+                      <c:ext uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                     </c:extLst>
                   </c15:dLbl>
                 </c15:categoryFilterException>
@@ -8000,11 +7982,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="-24"/>
-        <c:axId val="947163936"/>
-        <c:axId val="947162848"/>
+        <c:axId val="-1734623136"/>
+        <c:axId val="-1734622592"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="947163936"/>
+        <c:axId val="-1734623136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8046,7 +8028,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="947162848"/>
+        <c:crossAx val="-1734622592"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8054,7 +8036,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="947162848"/>
+        <c:axId val="-1734622592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8158,7 +8140,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="947163936"/>
+        <c:crossAx val="-1734623136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8993,11 +8975,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="-24"/>
-        <c:axId val="1815485328"/>
-        <c:axId val="1815486960"/>
+        <c:axId val="-1734621504"/>
+        <c:axId val="-1734636192"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1815485328"/>
+        <c:axId val="-1734621504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9039,7 +9021,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1815486960"/>
+        <c:crossAx val="-1734636192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9047,7 +9029,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1815486960"/>
+        <c:axId val="-1734636192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9151,7 +9133,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1815485328"/>
+        <c:crossAx val="-1734621504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10148,11 +10130,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="-24"/>
-        <c:axId val="1815476624"/>
-        <c:axId val="1815485872"/>
+        <c:axId val="-1734606816"/>
+        <c:axId val="-1734614976"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1815476624"/>
+        <c:axId val="-1734606816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10194,7 +10176,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1815485872"/>
+        <c:crossAx val="-1734614976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10202,7 +10184,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1815485872"/>
+        <c:axId val="-1734614976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10306,7 +10288,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1815476624"/>
+        <c:crossAx val="-1734606816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10570,11 +10552,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1725953808"/>
-        <c:axId val="1725954896"/>
+        <c:axId val="-1740102912"/>
+        <c:axId val="-1740101280"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1725953808"/>
+        <c:axId val="-1740102912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10592,7 +10574,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="1725954896"/>
+        <c:crossAx val="-1740101280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10600,7 +10582,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1725954896"/>
+        <c:axId val="-1740101280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10625,7 +10607,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="1725953808"/>
+        <c:crossAx val="-1740102912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.1"/>
@@ -10661,6 +10643,1179 @@
 </file>
 
 <file path=xl/charts/chart20.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$C$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Tahiti</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="00B050"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="95000"/>
+                          <a:alpha val="54000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Tabelle1!$B$6:$B$33</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Tabelle1!$B$9,Tabelle1!$B$12,Tabelle1!$B$15,Tabelle1!$B$18,Tabelle1!$B$21,Tabelle1!$B$33)</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Kernel 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Kernel 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Kernel 3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Kernel 4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Kernel 4.1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Reference</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Tabelle1!$C$6:$C$33</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Tabelle1!$C$9,Tabelle1!$C$12,Tabelle1!$C$15,Tabelle1!$C$18,Tabelle1!$C$21,Tabelle1!$C$33)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0" formatCode="0.00">
+                  <c:v>4.9249099999999997</c:v>
+                </c:pt>
+                <c:pt idx="1" formatCode="0.00">
+                  <c:v>5.2195049999999998</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="0.00">
+                  <c:v>3.4630000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0.00">
+                  <c:v>2.4160599999999999</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0.00">
+                  <c:v>4.8210899999999999</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="0.00">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$D$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Tesla</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ED7D31"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0"/>
+                  <c:y val="-2.0926885252835075E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="95000"/>
+                          <a:alpha val="54000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Tabelle1!$B$6:$B$33</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Tabelle1!$B$9,Tabelle1!$B$12,Tabelle1!$B$15,Tabelle1!$B$18,Tabelle1!$B$21,Tabelle1!$B$33)</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Kernel 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Kernel 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Kernel 3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Kernel 4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Kernel 4.1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Reference</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Tabelle1!$D$6:$D$33</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Tabelle1!$D$9,Tabelle1!$D$12,Tabelle1!$D$15,Tabelle1!$D$18,Tabelle1!$D$21,Tabelle1!$D$33)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0" formatCode="0.00">
+                  <c:v>0.21723400000000001</c:v>
+                </c:pt>
+                <c:pt idx="1" formatCode="0.00">
+                  <c:v>3.3380874999999999</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="0.00">
+                  <c:v>2.6963900000000001</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0.00">
+                  <c:v>2.8530249999999997</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0.00">
+                  <c:v>2.0138775</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="0.00">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$E$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Barts</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="C80000"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-3.9459022191400832E-17"/>
+                  <c:y val="-1.7439071044029187E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="95000"/>
+                          <a:alpha val="54000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Tabelle1!$B$6:$B$33</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Tabelle1!$B$9,Tabelle1!$B$12,Tabelle1!$B$15,Tabelle1!$B$18,Tabelle1!$B$21,Tabelle1!$B$33)</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Kernel 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Kernel 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Kernel 3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Kernel 4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Kernel 4.1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Reference</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Tabelle1!$E$6:$E$33</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Tabelle1!$E$9,Tabelle1!$E$12,Tabelle1!$E$15,Tabelle1!$E$18,Tabelle1!$E$21,Tabelle1!$E$33)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0" formatCode="0.00">
+                  <c:v>8.5662699999999994E-2</c:v>
+                </c:pt>
+                <c:pt idx="1" formatCode="0.00">
+                  <c:v>3.4301499999999998</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="0.00">
+                  <c:v>0.78665866666666673</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0.00">
+                  <c:v>1.7917025</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0.00">
+                  <c:v>2.47004</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="0.00">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$F$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Xeon</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="E2AC00"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0"/>
+                  <c:y val="-2.4776889544403446E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="95000"/>
+                          <a:alpha val="54000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Tabelle1!$B$6:$B$33</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Tabelle1!$B$9,Tabelle1!$B$12,Tabelle1!$B$15,Tabelle1!$B$18,Tabelle1!$B$21,Tabelle1!$B$33)</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Kernel 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Kernel 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Kernel 3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Kernel 4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Kernel 4.1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Reference</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Tabelle1!$F$6:$F$33</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Tabelle1!$F$9,Tabelle1!$F$12,Tabelle1!$F$15,Tabelle1!$F$18,Tabelle1!$F$21,Tabelle1!$F$33)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0" formatCode="0.00">
+                  <c:v>0.336335</c:v>
+                </c:pt>
+                <c:pt idx="1" formatCode="0.00">
+                  <c:v>0.94446533333333338</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="0.00">
+                  <c:v>0.3609093333333333</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0.00">
+                  <c:v>0.63453700000000002</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0.00">
+                  <c:v>0.7877926666666667</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="0.00">
+                  <c:v>0.11560533333333331</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$G$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Phenom II x6</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent5">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent5">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="95000"/>
+                          <a:alpha val="54000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Tabelle1!$B$6:$B$33</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Tabelle1!$B$9,Tabelle1!$B$12,Tabelle1!$B$15,Tabelle1!$B$18,Tabelle1!$B$21,Tabelle1!$B$33)</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Kernel 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Kernel 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Kernel 3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Kernel 4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Kernel 4.1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Reference</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Tabelle1!$G$6:$G$33</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Tabelle1!$G$9,Tabelle1!$G$12,Tabelle1!$G$15,Tabelle1!$G$18,Tabelle1!$G$21,Tabelle1!$G$33)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0" formatCode="0.00">
+                  <c:v>2.7745933333333334E-2</c:v>
+                </c:pt>
+                <c:pt idx="1" formatCode="0.00">
+                  <c:v>0.29635233333333333</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="0.00">
+                  <c:v>6.5944533333333333E-2</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0.00">
+                  <c:v>0.15054033333333333</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0.00">
+                  <c:v>0.24162733333333333</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="0.00">
+                  <c:v>3.2360066666666673E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="100"/>
+        <c:overlap val="-24"/>
+        <c:axId val="-1736389376"/>
+        <c:axId val="-1736382848"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-1736389376"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="54000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1736382848"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-1736382848"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>GSPS</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1736389376"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart21.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="de-DE"/>
@@ -11658,8 +12813,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1639822304"/>
-        <c:axId val="1639828832"/>
+        <c:axId val="-1734610080"/>
+        <c:axId val="-1734614432"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -12840,7 +13995,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1639822304"/>
+        <c:axId val="-1734610080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12876,7 +14031,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -12941,7 +14095,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1639828832"/>
+        <c:crossAx val="-1734614432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12949,7 +14103,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1639828832"/>
+        <c:axId val="-1734614432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="6"/>
@@ -12995,7 +14149,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -13054,7 +14207,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1639822304"/>
+        <c:crossAx val="-1734610080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:minorUnit val="0.5"/>
@@ -13069,7 +14222,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -13146,7 +14298,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart22.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="de-DE"/>
@@ -13161,7 +14313,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -14100,8 +15251,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="1639820128"/>
-        <c:axId val="1639817408"/>
+        <c:axId val="-1734611712"/>
+        <c:axId val="-1734606272"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredBarSeries>
@@ -15732,7 +16883,7 @@
         </c:extLst>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1639820128"/>
+        <c:axId val="-1734611712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15775,7 +16926,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1639817408"/>
+        <c:crossAx val="-1734606272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15783,7 +16934,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1639817408"/>
+        <c:axId val="-1734606272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5"/>
@@ -15835,7 +16986,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1639820128"/>
+        <c:crossAx val="-1734611712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -15849,7 +17000,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -16097,11 +17247,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1725964144"/>
-        <c:axId val="1725961968"/>
+        <c:axId val="-1740094752"/>
+        <c:axId val="-1740099104"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1725964144"/>
+        <c:axId val="-1740094752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16119,7 +17269,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="1725961968"/>
+        <c:crossAx val="-1740099104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -16127,7 +17277,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1725961968"/>
+        <c:axId val="-1740099104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16152,7 +17302,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="1725964144"/>
+        <c:crossAx val="-1740094752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -16852,11 +18002,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1725958704"/>
-        <c:axId val="1725959792"/>
+        <c:axId val="-1740095840"/>
+        <c:axId val="-1740094208"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1725958704"/>
+        <c:axId val="-1740095840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16874,7 +18024,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="1725959792"/>
+        <c:crossAx val="-1740094208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -16882,7 +18032,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1725959792"/>
+        <c:axId val="-1740094208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16907,7 +18057,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="1725958704"/>
+        <c:crossAx val="-1740095840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -17140,11 +18290,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1725964688"/>
-        <c:axId val="1725958160"/>
+        <c:axId val="-310218992"/>
+        <c:axId val="-310228240"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1725964688"/>
+        <c:axId val="-310218992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17162,7 +18312,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="1725958160"/>
+        <c:crossAx val="-310228240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -17170,7 +18320,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1725958160"/>
+        <c:axId val="-310228240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17195,7 +18345,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="1725964688"/>
+        <c:crossAx val="-310218992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.25"/>
@@ -17403,11 +18553,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1725951632"/>
-        <c:axId val="1725968496"/>
+        <c:axId val="-310215184"/>
+        <c:axId val="-310226608"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1725951632"/>
+        <c:axId val="-310215184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17425,7 +18575,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="1725968496"/>
+        <c:crossAx val="-310226608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -17433,7 +18583,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1725968496"/>
+        <c:axId val="-310226608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17458,7 +18608,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="1725951632"/>
+        <c:crossAx val="-310215184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.5"/>
@@ -17674,11 +18824,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1725966320"/>
-        <c:axId val="1725969040"/>
+        <c:axId val="-310227696"/>
+        <c:axId val="-310223888"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1725966320"/>
+        <c:axId val="-310227696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17696,7 +18846,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="1725969040"/>
+        <c:crossAx val="-310223888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -17704,7 +18854,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1725969040"/>
+        <c:axId val="-310223888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17729,7 +18879,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="1725966320"/>
+        <c:crossAx val="-310227696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.25"/>
@@ -18346,11 +19496,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1725970128"/>
-        <c:axId val="1725979920"/>
+        <c:axId val="-85599440"/>
+        <c:axId val="-85594544"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1725970128"/>
+        <c:axId val="-85599440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18368,7 +19518,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="1725979920"/>
+        <c:crossAx val="-85594544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -18376,7 +19526,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1725979920"/>
+        <c:axId val="-85594544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18401,7 +19551,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="1725970128"/>
+        <c:crossAx val="-85599440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -18635,8 +19785,8 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1725980464"/>
-        <c:axId val="1725971760"/>
+        <c:axId val="-87659984"/>
+        <c:axId val="-87657264"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredBarSeries>
@@ -19083,7 +20233,7 @@
         </c:extLst>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1725980464"/>
+        <c:axId val="-87659984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -19126,7 +20276,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1725971760"/>
+        <c:crossAx val="-87657264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -19134,7 +20284,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1725971760"/>
+        <c:axId val="-87657264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -19185,7 +20335,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1725980464"/>
+        <c:crossAx val="-87659984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="5"/>
@@ -19396,6 +20546,46 @@
 </file>
 
 <file path=xl/charts/colors13.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors14.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -21251,7 +22441,7 @@
 </file>
 
 <file path=xl/charts/style12.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="233">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="209">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -21273,11 +22463,11 @@
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="lt1">
             <a:lumMod val="95000"/>
-            <a:alpha val="10000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -21354,7 +22544,7 @@
     </cs:fillRef>
     <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
   </cs:dataPoint>
   <cs:dataPoint3D>
@@ -21364,7 +22554,7 @@
     </cs:fillRef>
     <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
   </cs:dataPoint3D>
   <cs:dataPointLine>
@@ -21374,7 +22564,7 @@
     <cs:fillRef idx="3"/>
     <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="34925" cap="rnd">
@@ -21394,7 +22584,7 @@
     </cs:fillRef>
     <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
@@ -21413,7 +22603,7 @@
     <cs:fillRef idx="3"/>
     <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -21450,7 +22640,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -21474,7 +22664,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
@@ -21493,7 +22683,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -21511,7 +22701,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
   </cs:floor>
   <cs:gridlineMajor>
@@ -21519,7 +22709,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -21538,7 +22728,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln>
@@ -21556,7 +22746,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
@@ -21575,7 +22765,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
@@ -21604,7 +22794,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
   </cs:plotArea>
   <cs:plotArea3D>
@@ -21612,7 +22802,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
   </cs:plotArea3D>
   <cs:seriesAxis>
@@ -21682,7 +22872,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="19050" cap="rnd">
@@ -21708,7 +22898,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -21740,13 +22930,509 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
 </file>
 
 <file path=xl/charts/style13.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="233">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style14.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -26835,6 +28521,38 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>147</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>42</xdr:col>
+      <xdr:colOff>91439</xdr:colOff>
+      <xdr:row>166</xdr:row>
+      <xdr:rowOff>149496</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="21" name="Diagramm 20"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId20"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -27168,8 +28886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:V151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y146" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="AJ159" sqref="AJ159"/>
+    <sheetView tabSelected="1" topLeftCell="AH147" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="AR163" sqref="AR163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>